<commit_message>
Add updated Excel template with fixed structure for import
- Bilanzdaten sheet is first (index 0) for auto-selection
- Headers written explicitly to prevent sparse arrays
- All 11 columns properly structured with 'Kontonummer' at column 2
- Verified structure matches import code requirements
</commit_message>
<xml_diff>
--- a/templates/Konsolidierung_Muster_v3.0.xlsx
+++ b/templates/Konsolidierung_Muster_v3.0.xlsx
@@ -7,8 +7,8 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Anleitung" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Bilanzdaten" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Bilanzdaten" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Anleitung1" sheetId="2" state="visible" r:id="rId2"/>
     <sheet name="GuV-Daten" sheetId="3" state="visible" r:id="rId3"/>
     <sheet name="Unternehmensinformationen" sheetId="4" state="visible" r:id="rId4"/>
     <sheet name="Beteiligungsverhältnisse" sheetId="5" state="visible" r:id="rId5"/>
@@ -18,6 +18,7 @@
     <sheet name="Latente Steuern" sheetId="9" state="visible" r:id="rId9"/>
     <sheet name="HGB-Bilanzstruktur" sheetId="10" state="visible" r:id="rId10"/>
     <sheet name="Kontenplan-Referenz" sheetId="11" state="visible" r:id="rId11"/>
+    <sheet name="Anleitung" sheetId="12" state="visible" r:id="rId12"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -41,6 +42,14 @@
     <font>
       <b val="1"/>
       <color rgb="00FFFFFF"/>
+      <sz val="11"/>
+    </font>
+    <font>
+      <b val="1"/>
+    </font>
+    <font>
+      <b val="1"/>
+      <color rgb="00FFFFFF"/>
       <sz val="16"/>
     </font>
     <font>
@@ -50,14 +59,6 @@
     <font>
       <b val="1"/>
       <sz val="12"/>
-    </font>
-    <font>
-      <b val="1"/>
-    </font>
-    <font>
-      <b val="1"/>
-      <color rgb="00FFFFFF"/>
-      <sz val="11"/>
     </font>
     <font>
       <b val="1"/>
@@ -117,15 +118,7 @@
   </cellStyleXfs>
   <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -136,10 +129,18 @@
     <xf numFmtId="4" fontId="0" fillId="4" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="4" fontId="4" fillId="4" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="4" fontId="2" fillId="4" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="4" fontId="4" fillId="4" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="4" fontId="2" fillId="4" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="4" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -147,7 +148,7 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -513,7 +514,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F41"/>
+  <dimension ref="A1:K16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -521,429 +522,812 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="20" customWidth="1" min="1" max="1"/>
-    <col width="60" customWidth="1" min="2" max="2"/>
+    <col width="25" customWidth="1" min="1" max="1"/>
+    <col width="15" customWidth="1" min="2" max="2"/>
+    <col width="30" customWidth="1" min="3" max="3"/>
+    <col width="15" customWidth="1" min="4" max="4"/>
+    <col width="15" customWidth="1" min="5" max="5"/>
+    <col width="15" customWidth="1" min="6" max="6"/>
+    <col width="15" customWidth="1" min="7" max="7"/>
+    <col width="15" customWidth="1" min="8" max="8"/>
+    <col width="20" customWidth="1" min="9" max="9"/>
+    <col width="20" customWidth="1" min="10" max="10"/>
+    <col width="40" customWidth="1" min="11" max="11"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>HGB-Konsolidierung Import-Template - Anleitung</t>
+          <t>Unternehmen</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Kontonummer</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Kontoname</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>HGB-Position</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Kontotyp</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Soll</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Haben</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Saldo</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Zwischengesellschaft</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Gegenpartei</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>Bemerkung</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Version 3.0 - Stand: 2026-01-14</t>
+          <t>Mutterunternehmen H</t>
+        </is>
+      </c>
+      <c r="B2" s="3" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+      <c r="C2" s="3" t="inlineStr">
+        <is>
+          <t>Kasse</t>
+        </is>
+      </c>
+      <c r="D2" s="3" t="inlineStr">
+        <is>
+          <t>B.IV</t>
+        </is>
+      </c>
+      <c r="E2" s="3" t="inlineStr">
+        <is>
+          <t>asset</t>
+        </is>
+      </c>
+      <c r="F2" s="4" t="inlineStr">
+        <is>
+          <t>5000.00</t>
+        </is>
+      </c>
+      <c r="G2" s="4" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="H2" s="5">
+        <f>F2-G2</f>
+        <v/>
+      </c>
+      <c r="I2" s="3" t="inlineStr">
+        <is>
+          <t>Nein</t>
+        </is>
+      </c>
+      <c r="J2" s="3" t="inlineStr"/>
+      <c r="K2" s="3" t="inlineStr"/>
+    </row>
+    <row r="3">
+      <c r="A3" s="2" t="inlineStr">
+        <is>
+          <t>Mutterunternehmen H</t>
+        </is>
+      </c>
+      <c r="B3" s="3" t="inlineStr">
+        <is>
+          <t>1200</t>
+        </is>
+      </c>
+      <c r="C3" s="3" t="inlineStr">
+        <is>
+          <t>Forderungen a. LL</t>
+        </is>
+      </c>
+      <c r="D3" s="3" t="inlineStr">
+        <is>
+          <t>B.II</t>
+        </is>
+      </c>
+      <c r="E3" s="3" t="inlineStr">
+        <is>
+          <t>asset</t>
+        </is>
+      </c>
+      <c r="F3" s="4" t="inlineStr">
+        <is>
+          <t>100000.00</t>
+        </is>
+      </c>
+      <c r="G3" s="4" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="H3" s="5">
+        <f>F3-G3</f>
+        <v/>
+      </c>
+      <c r="I3" s="3" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="J3" s="3" t="inlineStr">
+        <is>
+          <t>TU1</t>
+        </is>
+      </c>
+      <c r="K3" s="3" t="inlineStr">
+        <is>
+          <t>Zwischengesellschaftsgeschäft</t>
         </is>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="3" t="inlineStr">
-        <is>
-          <t>ÜBERSICHT DER BLÄTTER:</t>
+      <c r="A4" s="2" t="inlineStr">
+        <is>
+          <t>Mutterunternehmen H</t>
+        </is>
+      </c>
+      <c r="B4" s="3" t="inlineStr">
+        <is>
+          <t>1400</t>
+        </is>
+      </c>
+      <c r="C4" s="3" t="inlineStr">
+        <is>
+          <t>Beteiligung TU1</t>
+        </is>
+      </c>
+      <c r="D4" s="3" t="inlineStr">
+        <is>
+          <t>A.III</t>
+        </is>
+      </c>
+      <c r="E4" s="3" t="inlineStr">
+        <is>
+          <t>asset</t>
+        </is>
+      </c>
+      <c r="F4" s="4" t="inlineStr">
+        <is>
+          <t>500000.00</t>
+        </is>
+      </c>
+      <c r="G4" s="4" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="H4" s="5">
+        <f>F4-G4</f>
+        <v/>
+      </c>
+      <c r="I4" s="3" t="inlineStr">
+        <is>
+          <t>Nein</t>
+        </is>
+      </c>
+      <c r="J4" s="3" t="inlineStr"/>
+      <c r="K4" s="3" t="inlineStr">
+        <is>
+          <t>Beteiligung an Tochterunternehmen</t>
         </is>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="4" t="inlineStr">
-        <is>
-          <t>1. Anleitung</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>Dieses Blatt - Übersicht und Anleitung</t>
-        </is>
-      </c>
+      <c r="A5" s="2" t="inlineStr">
+        <is>
+          <t>Mutterunternehmen H</t>
+        </is>
+      </c>
+      <c r="B5" s="3" t="inlineStr">
+        <is>
+          <t>2000</t>
+        </is>
+      </c>
+      <c r="C5" s="3" t="inlineStr">
+        <is>
+          <t>Grundstücke</t>
+        </is>
+      </c>
+      <c r="D5" s="3" t="inlineStr">
+        <is>
+          <t>A.II</t>
+        </is>
+      </c>
+      <c r="E5" s="3" t="inlineStr">
+        <is>
+          <t>asset</t>
+        </is>
+      </c>
+      <c r="F5" s="4" t="inlineStr">
+        <is>
+          <t>2000000.00</t>
+        </is>
+      </c>
+      <c r="G5" s="4" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="H5" s="5">
+        <f>F5-G5</f>
+        <v/>
+      </c>
+      <c r="I5" s="3" t="inlineStr">
+        <is>
+          <t>Nein</t>
+        </is>
+      </c>
+      <c r="J5" s="3" t="inlineStr"/>
+      <c r="K5" s="3" t="inlineStr"/>
     </row>
     <row r="6">
-      <c r="A6" s="4" t="inlineStr">
-        <is>
-          <t>2. Bilanzdaten</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>Bilanzpositionen für alle Unternehmen (HGB § 266)</t>
-        </is>
-      </c>
+      <c r="A6" s="2" t="inlineStr">
+        <is>
+          <t>Mutterunternehmen H</t>
+        </is>
+      </c>
+      <c r="B6" s="3" t="inlineStr">
+        <is>
+          <t>3000</t>
+        </is>
+      </c>
+      <c r="C6" s="3" t="inlineStr">
+        <is>
+          <t>Gezeichnetes Kapital</t>
+        </is>
+      </c>
+      <c r="D6" s="3" t="inlineStr">
+        <is>
+          <t>A.I</t>
+        </is>
+      </c>
+      <c r="E6" s="3" t="inlineStr">
+        <is>
+          <t>equity</t>
+        </is>
+      </c>
+      <c r="F6" s="4" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="G6" s="4" t="inlineStr">
+        <is>
+          <t>1000000.00</t>
+        </is>
+      </c>
+      <c r="H6" s="5">
+        <f>F6-G6</f>
+        <v/>
+      </c>
+      <c r="I6" s="3" t="inlineStr">
+        <is>
+          <t>Nein</t>
+        </is>
+      </c>
+      <c r="J6" s="3" t="inlineStr"/>
+      <c r="K6" s="3" t="inlineStr"/>
     </row>
     <row r="7">
-      <c r="A7" s="4" t="inlineStr">
-        <is>
-          <t>3. GuV-Daten</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>Gewinn- und Verlustrechnung (HGB § 275)</t>
-        </is>
-      </c>
+      <c r="A7" s="2" t="inlineStr">
+        <is>
+          <t>Mutterunternehmen H</t>
+        </is>
+      </c>
+      <c r="B7" s="3" t="inlineStr">
+        <is>
+          <t>3100</t>
+        </is>
+      </c>
+      <c r="C7" s="3" t="inlineStr">
+        <is>
+          <t>Kapitalrücklage</t>
+        </is>
+      </c>
+      <c r="D7" s="3" t="inlineStr">
+        <is>
+          <t>A.II</t>
+        </is>
+      </c>
+      <c r="E7" s="3" t="inlineStr">
+        <is>
+          <t>equity</t>
+        </is>
+      </c>
+      <c r="F7" s="4" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="G7" s="4" t="inlineStr">
+        <is>
+          <t>200000.00</t>
+        </is>
+      </c>
+      <c r="H7" s="5">
+        <f>F7-G7</f>
+        <v/>
+      </c>
+      <c r="I7" s="3" t="inlineStr">
+        <is>
+          <t>Nein</t>
+        </is>
+      </c>
+      <c r="J7" s="3" t="inlineStr"/>
+      <c r="K7" s="3" t="inlineStr"/>
     </row>
     <row r="8">
-      <c r="A8" s="4" t="inlineStr">
-        <is>
-          <t>4. Unternehmensinformationen</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>Basis-Informationen zu allen Unternehmen</t>
-        </is>
-      </c>
+      <c r="A8" s="2" t="inlineStr">
+        <is>
+          <t>Mutterunternehmen H</t>
+        </is>
+      </c>
+      <c r="B8" s="3" t="inlineStr">
+        <is>
+          <t>3200</t>
+        </is>
+      </c>
+      <c r="C8" s="3" t="inlineStr">
+        <is>
+          <t>Gewinnrücklagen</t>
+        </is>
+      </c>
+      <c r="D8" s="3" t="inlineStr">
+        <is>
+          <t>A.III</t>
+        </is>
+      </c>
+      <c r="E8" s="3" t="inlineStr">
+        <is>
+          <t>equity</t>
+        </is>
+      </c>
+      <c r="F8" s="4" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="G8" s="4" t="inlineStr">
+        <is>
+          <t>300000.00</t>
+        </is>
+      </c>
+      <c r="H8" s="5">
+        <f>F8-G8</f>
+        <v/>
+      </c>
+      <c r="I8" s="3" t="inlineStr">
+        <is>
+          <t>Nein</t>
+        </is>
+      </c>
+      <c r="J8" s="3" t="inlineStr"/>
+      <c r="K8" s="3" t="inlineStr"/>
     </row>
     <row r="9">
-      <c r="A9" s="4" t="inlineStr">
-        <is>
-          <t>5. Beteiligungsverhältnisse</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>Für Kapitalkonsolidierung (HGB § 301)</t>
-        </is>
-      </c>
+      <c r="A9" s="2" t="inlineStr">
+        <is>
+          <t>Mutterunternehmen H</t>
+        </is>
+      </c>
+      <c r="B9" s="3" t="inlineStr">
+        <is>
+          <t>4000</t>
+        </is>
+      </c>
+      <c r="C9" s="3" t="inlineStr">
+        <is>
+          <t>Verbindlichkeiten</t>
+        </is>
+      </c>
+      <c r="D9" s="3" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="E9" s="3" t="inlineStr">
+        <is>
+          <t>liability</t>
+        </is>
+      </c>
+      <c r="F9" s="4" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="G9" s="4" t="inlineStr">
+        <is>
+          <t>500000.00</t>
+        </is>
+      </c>
+      <c r="H9" s="5">
+        <f>F9-G9</f>
+        <v/>
+      </c>
+      <c r="I9" s="3" t="inlineStr">
+        <is>
+          <t>Nein</t>
+        </is>
+      </c>
+      <c r="J9" s="3" t="inlineStr"/>
+      <c r="K9" s="3" t="inlineStr"/>
     </row>
     <row r="10">
-      <c r="A10" s="4" t="inlineStr">
-        <is>
-          <t>6. Zwischengesellschaftsgeschäfte</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>Für Schulden- und Zwischenergebniseliminierung (HGB § 303, § 305)</t>
-        </is>
-      </c>
+      <c r="A10" s="2" t="inlineStr">
+        <is>
+          <t>Tochterunternehmen TU1</t>
+        </is>
+      </c>
+      <c r="B10" s="3" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+      <c r="C10" s="3" t="inlineStr">
+        <is>
+          <t>Kasse</t>
+        </is>
+      </c>
+      <c r="D10" s="3" t="inlineStr">
+        <is>
+          <t>B.IV</t>
+        </is>
+      </c>
+      <c r="E10" s="3" t="inlineStr">
+        <is>
+          <t>asset</t>
+        </is>
+      </c>
+      <c r="F10" s="4" t="inlineStr">
+        <is>
+          <t>2000.00</t>
+        </is>
+      </c>
+      <c r="G10" s="4" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="H10" s="5">
+        <f>F10-G10</f>
+        <v/>
+      </c>
+      <c r="I10" s="3" t="inlineStr">
+        <is>
+          <t>Nein</t>
+        </is>
+      </c>
+      <c r="J10" s="3" t="inlineStr"/>
+      <c r="K10" s="3" t="inlineStr"/>
     </row>
     <row r="11">
-      <c r="A11" s="4" t="inlineStr">
-        <is>
-          <t>7. Eigenkapital-Aufteilung</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>Für Minderheitsanteile</t>
+      <c r="A11" s="2" t="inlineStr">
+        <is>
+          <t>Tochterunternehmen TU1</t>
+        </is>
+      </c>
+      <c r="B11" s="3" t="inlineStr">
+        <is>
+          <t>1600</t>
+        </is>
+      </c>
+      <c r="C11" s="3" t="inlineStr">
+        <is>
+          <t>Verbindlichkeiten a. LL</t>
+        </is>
+      </c>
+      <c r="D11" s="3" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="E11" s="3" t="inlineStr">
+        <is>
+          <t>liability</t>
+        </is>
+      </c>
+      <c r="F11" s="4" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="G11" s="4" t="inlineStr">
+        <is>
+          <t>50000.00</t>
+        </is>
+      </c>
+      <c r="H11" s="5">
+        <f>F11-G11</f>
+        <v/>
+      </c>
+      <c r="I11" s="3" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="J11" s="3" t="inlineStr">
+        <is>
+          <t>Mutter H</t>
+        </is>
+      </c>
+      <c r="K11" s="3" t="inlineStr">
+        <is>
+          <t>Gegenpartei: Mutterunternehmen H</t>
         </is>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="4" t="inlineStr">
-        <is>
-          <t>8. Währungsumrechnung</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>Für ausländische Tochterunternehmen (HGB § 256a) - NEU</t>
-        </is>
-      </c>
+      <c r="A12" s="2" t="inlineStr">
+        <is>
+          <t>Tochterunternehmen TU1</t>
+        </is>
+      </c>
+      <c r="B12" s="3" t="inlineStr">
+        <is>
+          <t>3000</t>
+        </is>
+      </c>
+      <c r="C12" s="3" t="inlineStr">
+        <is>
+          <t>Gezeichnetes Kapital</t>
+        </is>
+      </c>
+      <c r="D12" s="3" t="inlineStr">
+        <is>
+          <t>A.I</t>
+        </is>
+      </c>
+      <c r="E12" s="3" t="inlineStr">
+        <is>
+          <t>equity</t>
+        </is>
+      </c>
+      <c r="F12" s="4" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="G12" s="4" t="inlineStr">
+        <is>
+          <t>500000.00</t>
+        </is>
+      </c>
+      <c r="H12" s="5">
+        <f>F12-G12</f>
+        <v/>
+      </c>
+      <c r="I12" s="3" t="inlineStr">
+        <is>
+          <t>Nein</t>
+        </is>
+      </c>
+      <c r="J12" s="3" t="inlineStr"/>
+      <c r="K12" s="3" t="inlineStr"/>
     </row>
     <row r="13">
-      <c r="A13" s="4" t="inlineStr">
-        <is>
-          <t>9. Latente Steuern</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>Aktive und passive latente Steuern (HGB § 274) - NEU</t>
-        </is>
-      </c>
+      <c r="A13" s="2" t="inlineStr">
+        <is>
+          <t>Tochterunternehmen TU2</t>
+        </is>
+      </c>
+      <c r="B13" s="3" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+      <c r="C13" s="3" t="inlineStr">
+        <is>
+          <t>Kasse</t>
+        </is>
+      </c>
+      <c r="D13" s="3" t="inlineStr">
+        <is>
+          <t>B.IV</t>
+        </is>
+      </c>
+      <c r="E13" s="3" t="inlineStr">
+        <is>
+          <t>asset</t>
+        </is>
+      </c>
+      <c r="F13" s="4" t="inlineStr">
+        <is>
+          <t>1500.00</t>
+        </is>
+      </c>
+      <c r="G13" s="4" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="H13" s="5">
+        <f>F13-G13</f>
+        <v/>
+      </c>
+      <c r="I13" s="3" t="inlineStr">
+        <is>
+          <t>Nein</t>
+        </is>
+      </c>
+      <c r="J13" s="3" t="inlineStr"/>
+      <c r="K13" s="3" t="inlineStr"/>
     </row>
     <row r="14">
-      <c r="A14" s="4" t="inlineStr">
-        <is>
-          <t>10. HGB-Bilanzstruktur</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>Referenz zur HGB-Bilanzgliederung (HGB § 266)</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" s="4" t="inlineStr">
-        <is>
-          <t>11. Kontenplan-Referenz</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>Typische Kontonummern-Bereiche</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" s="3" t="inlineStr">
-        <is>
-          <t>SCHRITT-FÜR-SCHRITT-ANLEITUNG:</t>
-        </is>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" s="4" t="inlineStr">
-        <is>
-          <t>Schritt 1:</t>
-        </is>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>Füllen Sie 'Unternehmensinformationen' aus</t>
-        </is>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" s="4" t="inlineStr">
-        <is>
-          <t>Schritt 2:</t>
-        </is>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>Füllen Sie 'Bilanzdaten' für alle Unternehmen aus</t>
-        </is>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" s="4" t="inlineStr">
-        <is>
-          <t>Schritt 3:</t>
-        </is>
-      </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>Füllen Sie 'GuV-Daten' für alle Unternehmen aus</t>
-        </is>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" s="4" t="inlineStr">
-        <is>
-          <t>Schritt 4:</t>
-        </is>
-      </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>Definieren Sie 'Beteiligungsverhältnisse'</t>
-        </is>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" s="4" t="inlineStr">
-        <is>
-          <t>Schritt 5:</t>
-        </is>
-      </c>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>Erfassen Sie alle 'Zwischengesellschaftsgeschäfte'</t>
-        </is>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" s="4" t="inlineStr">
-        <is>
-          <t>Schritt 6:</t>
-        </is>
-      </c>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>Prüfen Sie 'Eigenkapital-Aufteilung'</t>
-        </is>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" s="4" t="inlineStr">
-        <is>
-          <t>Schritt 7:</t>
-        </is>
-      </c>
-      <c r="B24" t="inlineStr">
-        <is>
-          <t>Bei ausländischen Unternehmen: 'Währungsumrechnung' ausfüllen</t>
-        </is>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" s="4" t="inlineStr">
-        <is>
-          <t>Schritt 8:</t>
-        </is>
-      </c>
-      <c r="B25" t="inlineStr">
-        <is>
-          <t>Bei Steuerdifferenzen: 'Latente Steuern' ausfüllen</t>
-        </is>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" s="4" t="inlineStr">
-        <is>
-          <t>Schritt 9:</t>
-        </is>
-      </c>
-      <c r="B26" t="inlineStr">
-        <is>
-          <t>Importieren Sie die Datei im System</t>
-        </is>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" s="3" t="inlineStr">
-        <is>
-          <t>HGB-REFERENZEN:</t>
-        </is>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" s="4" t="inlineStr">
-        <is>
-          <t>§ 266 HGB</t>
-        </is>
-      </c>
-      <c r="B29" t="inlineStr">
-        <is>
-          <t>Bilanzgliederung</t>
-        </is>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" s="4" t="inlineStr">
-        <is>
-          <t>§ 275 HGB</t>
-        </is>
-      </c>
-      <c r="B30" t="inlineStr">
-        <is>
-          <t>Gewinn- und Verlustrechnung</t>
-        </is>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" s="4" t="inlineStr">
-        <is>
-          <t>§ 301 HGB</t>
-        </is>
-      </c>
-      <c r="B31" t="inlineStr">
-        <is>
-          <t>Kapitalkonsolidierung</t>
-        </is>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" s="4" t="inlineStr">
-        <is>
-          <t>§ 303 HGB</t>
-        </is>
-      </c>
-      <c r="B32" t="inlineStr">
-        <is>
-          <t>Schuldenkonsolidierung</t>
-        </is>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" s="4" t="inlineStr">
-        <is>
-          <t>§ 305 HGB</t>
-        </is>
-      </c>
-      <c r="B33" t="inlineStr">
-        <is>
-          <t>Zwischenergebniseliminierung</t>
-        </is>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" s="4" t="inlineStr">
-        <is>
-          <t>§ 274 HGB</t>
-        </is>
-      </c>
-      <c r="B34" t="inlineStr">
-        <is>
-          <t>Latente Steuern</t>
-        </is>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" s="4" t="inlineStr">
-        <is>
-          <t>§ 256a HGB</t>
-        </is>
-      </c>
-      <c r="B35" t="inlineStr">
-        <is>
-          <t>Währungsumrechnung</t>
-        </is>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37" s="3" t="inlineStr">
-        <is>
-          <t>FARBCODierung:</t>
-        </is>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" s="4" t="inlineStr">
-        <is>
-          <t>Blau</t>
-        </is>
-      </c>
-      <c r="B38" t="inlineStr">
-        <is>
-          <t>Pflichtfelder (müssen ausgefüllt werden)</t>
-        </is>
-      </c>
-    </row>
-    <row r="39">
-      <c r="A39" s="4" t="inlineStr">
-        <is>
-          <t>Gelb</t>
-        </is>
-      </c>
-      <c r="B39" t="inlineStr">
-        <is>
-          <t>Optionale Felder</t>
-        </is>
-      </c>
-    </row>
-    <row r="40">
-      <c r="A40" s="4" t="inlineStr">
-        <is>
-          <t>Grün</t>
-        </is>
-      </c>
-      <c r="B40" t="inlineStr">
-        <is>
-          <t>Berechnete Felder (Formeln)</t>
-        </is>
-      </c>
-    </row>
-    <row r="41">
-      <c r="A41" s="4" t="inlineStr">
-        <is>
-          <t>Rot</t>
-        </is>
-      </c>
-      <c r="B41" t="inlineStr">
-        <is>
-          <t>Warnungen/Hinweise</t>
-        </is>
+      <c r="A14" s="2" t="inlineStr">
+        <is>
+          <t>Tochterunternehmen TU2</t>
+        </is>
+      </c>
+      <c r="B14" s="3" t="inlineStr">
+        <is>
+          <t>3000</t>
+        </is>
+      </c>
+      <c r="C14" s="3" t="inlineStr">
+        <is>
+          <t>Gezeichnetes Kapital</t>
+        </is>
+      </c>
+      <c r="D14" s="3" t="inlineStr">
+        <is>
+          <t>A.I</t>
+        </is>
+      </c>
+      <c r="E14" s="3" t="inlineStr">
+        <is>
+          <t>equity</t>
+        </is>
+      </c>
+      <c r="F14" s="4" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="G14" s="4" t="inlineStr">
+        <is>
+          <t>300000.00</t>
+        </is>
+      </c>
+      <c r="H14" s="5">
+        <f>F14-G14</f>
+        <v/>
+      </c>
+      <c r="I14" s="3" t="inlineStr">
+        <is>
+          <t>Nein</t>
+        </is>
+      </c>
+      <c r="J14" s="3" t="inlineStr"/>
+      <c r="K14" s="3" t="inlineStr"/>
+    </row>
+    <row r="16">
+      <c r="A16" s="6" t="inlineStr">
+        <is>
+          <t>BILANZSUMME</t>
+        </is>
+      </c>
+      <c r="H16" s="7">
+        <f>SUM(H2:H14)</f>
+        <v/>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A2:F2"/>
-    <mergeCell ref="A1:F1"/>
-  </mergeCells>
+  <dataValidations count="26">
+    <dataValidation sqref="E2" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
+      <formula1>"asset,liability,equity"</formula1>
+    </dataValidation>
+    <dataValidation sqref="I2" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
+      <formula1>"Ja,Nein"</formula1>
+    </dataValidation>
+    <dataValidation sqref="E3" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
+      <formula1>"asset,liability,equity"</formula1>
+    </dataValidation>
+    <dataValidation sqref="I3" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
+      <formula1>"Ja,Nein"</formula1>
+    </dataValidation>
+    <dataValidation sqref="E4" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
+      <formula1>"asset,liability,equity"</formula1>
+    </dataValidation>
+    <dataValidation sqref="I4" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
+      <formula1>"Ja,Nein"</formula1>
+    </dataValidation>
+    <dataValidation sqref="E5" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
+      <formula1>"asset,liability,equity"</formula1>
+    </dataValidation>
+    <dataValidation sqref="I5" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
+      <formula1>"Ja,Nein"</formula1>
+    </dataValidation>
+    <dataValidation sqref="E6" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
+      <formula1>"asset,liability,equity"</formula1>
+    </dataValidation>
+    <dataValidation sqref="I6" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
+      <formula1>"Ja,Nein"</formula1>
+    </dataValidation>
+    <dataValidation sqref="E7" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
+      <formula1>"asset,liability,equity"</formula1>
+    </dataValidation>
+    <dataValidation sqref="I7" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
+      <formula1>"Ja,Nein"</formula1>
+    </dataValidation>
+    <dataValidation sqref="E8" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
+      <formula1>"asset,liability,equity"</formula1>
+    </dataValidation>
+    <dataValidation sqref="I8" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
+      <formula1>"Ja,Nein"</formula1>
+    </dataValidation>
+    <dataValidation sqref="E9" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
+      <formula1>"asset,liability,equity"</formula1>
+    </dataValidation>
+    <dataValidation sqref="I9" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
+      <formula1>"Ja,Nein"</formula1>
+    </dataValidation>
+    <dataValidation sqref="E10" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
+      <formula1>"asset,liability,equity"</formula1>
+    </dataValidation>
+    <dataValidation sqref="I10" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
+      <formula1>"Ja,Nein"</formula1>
+    </dataValidation>
+    <dataValidation sqref="E11" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
+      <formula1>"asset,liability,equity"</formula1>
+    </dataValidation>
+    <dataValidation sqref="I11" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
+      <formula1>"Ja,Nein"</formula1>
+    </dataValidation>
+    <dataValidation sqref="E12" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
+      <formula1>"asset,liability,equity"</formula1>
+    </dataValidation>
+    <dataValidation sqref="I12" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
+      <formula1>"Ja,Nein"</formula1>
+    </dataValidation>
+    <dataValidation sqref="E13" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
+      <formula1>"asset,liability,equity"</formula1>
+    </dataValidation>
+    <dataValidation sqref="I13" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
+      <formula1>"Ja,Nein"</formula1>
+    </dataValidation>
+    <dataValidation sqref="E14" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
+      <formula1>"asset,liability,equity"</formula1>
+    </dataValidation>
+    <dataValidation sqref="I14" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
+      <formula1>"Ja,Nein"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -975,7 +1359,7 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="3" t="inlineStr">
+      <c r="A3" s="10" t="inlineStr">
         <is>
           <t>AKTIVSEITE</t>
         </is>
@@ -1097,7 +1481,7 @@
       <c r="C14" t="inlineStr"/>
     </row>
     <row r="16">
-      <c r="A16" s="3" t="inlineStr">
+      <c r="A16" s="10" t="inlineStr">
         <is>
           <t>PASSIVSEITE</t>
         </is>
@@ -1249,264 +1633,264 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="5" t="inlineStr">
+      <c r="A2" s="1" t="inlineStr">
         <is>
           <t>Kontonummer-Bereich</t>
         </is>
       </c>
-      <c r="B2" s="5" t="inlineStr">
+      <c r="B2" s="1" t="inlineStr">
         <is>
           <t>Kontotyp</t>
         </is>
       </c>
-      <c r="C2" s="5" t="inlineStr">
+      <c r="C2" s="1" t="inlineStr">
         <is>
           <t>Beschreibung</t>
         </is>
       </c>
-      <c r="D2" s="5" t="inlineStr">
+      <c r="D2" s="1" t="inlineStr">
         <is>
           <t>HGB-Position</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="7" t="inlineStr">
+      <c r="A3" s="3" t="inlineStr">
         <is>
           <t>0000-0999</t>
         </is>
       </c>
-      <c r="B3" s="7" t="inlineStr">
+      <c r="B3" s="3" t="inlineStr">
         <is>
           <t>asset</t>
         </is>
       </c>
-      <c r="C3" s="7" t="inlineStr">
+      <c r="C3" s="3" t="inlineStr">
         <is>
           <t>Anlagevermögen (Immaterielle Vermögensgegenstände)</t>
         </is>
       </c>
-      <c r="D3" s="7" t="inlineStr">
+      <c r="D3" s="3" t="inlineStr">
         <is>
           <t>A.I</t>
         </is>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="7" t="inlineStr">
+      <c r="A4" s="3" t="inlineStr">
         <is>
           <t>1000-1499</t>
         </is>
       </c>
-      <c r="B4" s="7" t="inlineStr">
+      <c r="B4" s="3" t="inlineStr">
         <is>
           <t>asset</t>
         </is>
       </c>
-      <c r="C4" s="7" t="inlineStr">
+      <c r="C4" s="3" t="inlineStr">
         <is>
           <t>Anlagevermögen (Sachanlagen, Finanzanlagen)</t>
         </is>
       </c>
-      <c r="D4" s="7" t="inlineStr">
+      <c r="D4" s="3" t="inlineStr">
         <is>
           <t>A.II, A.III</t>
         </is>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="7" t="inlineStr">
+      <c r="A5" s="3" t="inlineStr">
         <is>
           <t>1500-1999</t>
         </is>
       </c>
-      <c r="B5" s="7" t="inlineStr">
+      <c r="B5" s="3" t="inlineStr">
         <is>
           <t>asset</t>
         </is>
       </c>
-      <c r="C5" s="7" t="inlineStr">
+      <c r="C5" s="3" t="inlineStr">
         <is>
           <t>Umlaufvermögen (Vorräte, Forderungen)</t>
         </is>
       </c>
-      <c r="D5" s="7" t="inlineStr">
+      <c r="D5" s="3" t="inlineStr">
         <is>
           <t>B.I, B.II</t>
         </is>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="7" t="inlineStr">
+      <c r="A6" s="3" t="inlineStr">
         <is>
           <t>2000-2999</t>
         </is>
       </c>
-      <c r="B6" s="7" t="inlineStr">
+      <c r="B6" s="3" t="inlineStr">
         <is>
           <t>asset</t>
         </is>
       </c>
-      <c r="C6" s="7" t="inlineStr">
+      <c r="C6" s="3" t="inlineStr">
         <is>
           <t>Umlaufvermögen (Wertpapiere, Kasse, Bank)</t>
         </is>
       </c>
-      <c r="D6" s="7" t="inlineStr">
+      <c r="D6" s="3" t="inlineStr">
         <is>
           <t>B.III, B.IV</t>
         </is>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="7" t="inlineStr">
+      <c r="A7" s="3" t="inlineStr">
         <is>
           <t>3000-3999</t>
         </is>
       </c>
-      <c r="B7" s="7" t="inlineStr">
+      <c r="B7" s="3" t="inlineStr">
         <is>
           <t>equity</t>
         </is>
       </c>
-      <c r="C7" s="7" t="inlineStr">
+      <c r="C7" s="3" t="inlineStr">
         <is>
           <t>Eigenkapital</t>
         </is>
       </c>
-      <c r="D7" s="7" t="inlineStr">
+      <c r="D7" s="3" t="inlineStr">
         <is>
           <t>A</t>
         </is>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="7" t="inlineStr">
+      <c r="A8" s="3" t="inlineStr">
         <is>
           <t>4000-4999</t>
         </is>
       </c>
-      <c r="B8" s="7" t="inlineStr">
+      <c r="B8" s="3" t="inlineStr">
         <is>
           <t>liability</t>
         </is>
       </c>
-      <c r="C8" s="7" t="inlineStr">
+      <c r="C8" s="3" t="inlineStr">
         <is>
           <t>Verbindlichkeiten</t>
         </is>
       </c>
-      <c r="D8" s="7" t="inlineStr">
+      <c r="D8" s="3" t="inlineStr">
         <is>
           <t>C</t>
         </is>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="7" t="inlineStr">
+      <c r="A9" s="3" t="inlineStr">
         <is>
           <t>5000-5999</t>
         </is>
       </c>
-      <c r="B9" s="7" t="inlineStr">
+      <c r="B9" s="3" t="inlineStr">
         <is>
           <t>liability</t>
         </is>
       </c>
-      <c r="C9" s="7" t="inlineStr">
+      <c r="C9" s="3" t="inlineStr">
         <is>
           <t>Rückstellungen</t>
         </is>
       </c>
-      <c r="D9" s="7" t="inlineStr">
+      <c r="D9" s="3" t="inlineStr">
         <is>
           <t>B</t>
         </is>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="7" t="inlineStr">
+      <c r="A10" s="3" t="inlineStr">
         <is>
           <t>6000-6999</t>
         </is>
       </c>
-      <c r="B10" s="7" t="inlineStr">
+      <c r="B10" s="3" t="inlineStr">
         <is>
           <t>expense</t>
         </is>
       </c>
-      <c r="C10" s="7" t="inlineStr">
+      <c r="C10" s="3" t="inlineStr">
         <is>
           <t>Aufwendungen (Material, Personal)</t>
         </is>
       </c>
-      <c r="D10" s="7" t="inlineStr">
+      <c r="D10" s="3" t="inlineStr">
         <is>
           <t>GuV</t>
         </is>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="7" t="inlineStr">
+      <c r="A11" s="3" t="inlineStr">
         <is>
           <t>7000-7999</t>
         </is>
       </c>
-      <c r="B11" s="7" t="inlineStr">
+      <c r="B11" s="3" t="inlineStr">
         <is>
           <t>expense</t>
         </is>
       </c>
-      <c r="C11" s="7" t="inlineStr">
+      <c r="C11" s="3" t="inlineStr">
         <is>
           <t>Aufwendungen (Abschreibungen, Zinsen)</t>
         </is>
       </c>
-      <c r="D11" s="7" t="inlineStr">
+      <c r="D11" s="3" t="inlineStr">
         <is>
           <t>GuV</t>
         </is>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="7" t="inlineStr">
+      <c r="A12" s="3" t="inlineStr">
         <is>
           <t>8000-8999</t>
         </is>
       </c>
-      <c r="B12" s="7" t="inlineStr">
+      <c r="B12" s="3" t="inlineStr">
         <is>
           <t>revenue</t>
         </is>
       </c>
-      <c r="C12" s="7" t="inlineStr">
+      <c r="C12" s="3" t="inlineStr">
         <is>
           <t>Erträge (Umsatzerlöse, sonstige Erträge)</t>
         </is>
       </c>
-      <c r="D12" s="7" t="inlineStr">
+      <c r="D12" s="3" t="inlineStr">
         <is>
           <t>GuV</t>
         </is>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="7" t="inlineStr">
+      <c r="A13" s="3" t="inlineStr">
         <is>
           <t>9000-9999</t>
         </is>
       </c>
-      <c r="B13" s="7" t="inlineStr">
+      <c r="B13" s="3" t="inlineStr">
         <is>
           <t>equity</t>
         </is>
       </c>
-      <c r="C13" s="7" t="inlineStr">
+      <c r="C13" s="3" t="inlineStr">
         <is>
           <t>GuV-Abschluss</t>
         </is>
       </c>
-      <c r="D13" s="7" t="inlineStr">
+      <c r="D13" s="3" t="inlineStr">
         <is>
           <t>A.V</t>
         </is>
@@ -1516,6 +1900,24 @@
   <mergeCells count="1">
     <mergeCell ref="A1:D1"/>
   </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -1526,7 +1928,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K16"/>
+  <dimension ref="A1:F41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1534,812 +1936,429 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="25" customWidth="1" min="1" max="1"/>
-    <col width="15" customWidth="1" min="2" max="2"/>
-    <col width="30" customWidth="1" min="3" max="3"/>
-    <col width="15" customWidth="1" min="4" max="4"/>
-    <col width="15" customWidth="1" min="5" max="5"/>
-    <col width="15" customWidth="1" min="6" max="6"/>
-    <col width="15" customWidth="1" min="7" max="7"/>
-    <col width="15" customWidth="1" min="8" max="8"/>
-    <col width="20" customWidth="1" min="9" max="9"/>
-    <col width="20" customWidth="1" min="10" max="10"/>
-    <col width="40" customWidth="1" min="11" max="11"/>
+    <col width="20" customWidth="1" min="1" max="1"/>
+    <col width="60" customWidth="1" min="2" max="2"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="5" t="inlineStr">
-        <is>
-          <t>Unternehmen</t>
-        </is>
-      </c>
-      <c r="B1" s="5" t="inlineStr">
-        <is>
-          <t>Kontonummer</t>
-        </is>
-      </c>
-      <c r="C1" s="5" t="inlineStr">
-        <is>
-          <t>Kontoname</t>
-        </is>
-      </c>
-      <c r="D1" s="5" t="inlineStr">
-        <is>
-          <t>HGB-Position</t>
-        </is>
-      </c>
-      <c r="E1" s="5" t="inlineStr">
-        <is>
-          <t>Kontotyp</t>
-        </is>
-      </c>
-      <c r="F1" s="5" t="inlineStr">
-        <is>
-          <t>Soll</t>
-        </is>
-      </c>
-      <c r="G1" s="5" t="inlineStr">
-        <is>
-          <t>Haben</t>
-        </is>
-      </c>
-      <c r="H1" s="5" t="inlineStr">
-        <is>
-          <t>Saldo</t>
-        </is>
-      </c>
-      <c r="I1" s="5" t="inlineStr">
-        <is>
-          <t>Zwischengesellschaft</t>
-        </is>
-      </c>
-      <c r="J1" s="5" t="inlineStr">
-        <is>
-          <t>Gegenpartei</t>
-        </is>
-      </c>
-      <c r="K1" s="5" t="inlineStr">
-        <is>
-          <t>Bemerkung</t>
+      <c r="A1" s="8" t="inlineStr">
+        <is>
+          <t>HGB-Konsolidierung Import-Template - Anleitung</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="6" t="inlineStr">
-        <is>
-          <t>Mutterunternehmen H</t>
-        </is>
-      </c>
-      <c r="B2" s="7" t="inlineStr">
-        <is>
-          <t>1000</t>
-        </is>
-      </c>
-      <c r="C2" s="7" t="inlineStr">
-        <is>
-          <t>Kasse</t>
-        </is>
-      </c>
-      <c r="D2" s="7" t="inlineStr">
-        <is>
-          <t>B.IV</t>
-        </is>
-      </c>
-      <c r="E2" s="7" t="inlineStr">
-        <is>
-          <t>asset</t>
-        </is>
-      </c>
-      <c r="F2" s="8" t="inlineStr">
-        <is>
-          <t>5000.00</t>
-        </is>
-      </c>
-      <c r="G2" s="8" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
-      </c>
-      <c r="H2" s="9">
-        <f>F2-G2</f>
-        <v/>
-      </c>
-      <c r="I2" s="7" t="inlineStr">
-        <is>
-          <t>Nein</t>
-        </is>
-      </c>
-      <c r="J2" s="7" t="inlineStr"/>
-      <c r="K2" s="7" t="inlineStr"/>
-    </row>
-    <row r="3">
-      <c r="A3" s="6" t="inlineStr">
-        <is>
-          <t>Mutterunternehmen H</t>
-        </is>
-      </c>
-      <c r="B3" s="7" t="inlineStr">
-        <is>
-          <t>1200</t>
-        </is>
-      </c>
-      <c r="C3" s="7" t="inlineStr">
-        <is>
-          <t>Forderungen a. LL</t>
-        </is>
-      </c>
-      <c r="D3" s="7" t="inlineStr">
-        <is>
-          <t>B.II</t>
-        </is>
-      </c>
-      <c r="E3" s="7" t="inlineStr">
-        <is>
-          <t>asset</t>
-        </is>
-      </c>
-      <c r="F3" s="8" t="inlineStr">
-        <is>
-          <t>100000.00</t>
-        </is>
-      </c>
-      <c r="G3" s="8" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
-      </c>
-      <c r="H3" s="9">
-        <f>F3-G3</f>
-        <v/>
-      </c>
-      <c r="I3" s="7" t="inlineStr">
-        <is>
-          <t>Ja</t>
-        </is>
-      </c>
-      <c r="J3" s="7" t="inlineStr">
-        <is>
-          <t>TU1</t>
-        </is>
-      </c>
-      <c r="K3" s="7" t="inlineStr">
-        <is>
-          <t>Zwischengesellschaftsgeschäft</t>
+      <c r="A2" s="9" t="inlineStr">
+        <is>
+          <t>Version 3.0 - Stand: 2026-01-15</t>
         </is>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="6" t="inlineStr">
-        <is>
-          <t>Mutterunternehmen H</t>
-        </is>
-      </c>
-      <c r="B4" s="7" t="inlineStr">
-        <is>
-          <t>1400</t>
-        </is>
-      </c>
-      <c r="C4" s="7" t="inlineStr">
-        <is>
-          <t>Beteiligung TU1</t>
-        </is>
-      </c>
-      <c r="D4" s="7" t="inlineStr">
-        <is>
-          <t>A.III</t>
-        </is>
-      </c>
-      <c r="E4" s="7" t="inlineStr">
-        <is>
-          <t>asset</t>
-        </is>
-      </c>
-      <c r="F4" s="8" t="inlineStr">
-        <is>
-          <t>500000.00</t>
-        </is>
-      </c>
-      <c r="G4" s="8" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
-      </c>
-      <c r="H4" s="9">
-        <f>F4-G4</f>
-        <v/>
-      </c>
-      <c r="I4" s="7" t="inlineStr">
-        <is>
-          <t>Nein</t>
-        </is>
-      </c>
-      <c r="J4" s="7" t="inlineStr"/>
-      <c r="K4" s="7" t="inlineStr">
-        <is>
-          <t>Beteiligung an Tochterunternehmen</t>
+      <c r="A4" s="10" t="inlineStr">
+        <is>
+          <t>ÜBERSICHT DER BLÄTTER:</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="6" t="inlineStr">
         <is>
-          <t>Mutterunternehmen H</t>
-        </is>
-      </c>
-      <c r="B5" s="7" t="inlineStr">
-        <is>
-          <t>2000</t>
-        </is>
-      </c>
-      <c r="C5" s="7" t="inlineStr">
-        <is>
-          <t>Grundstücke</t>
-        </is>
-      </c>
-      <c r="D5" s="7" t="inlineStr">
-        <is>
-          <t>A.II</t>
-        </is>
-      </c>
-      <c r="E5" s="7" t="inlineStr">
-        <is>
-          <t>asset</t>
-        </is>
-      </c>
-      <c r="F5" s="8" t="inlineStr">
-        <is>
-          <t>2000000.00</t>
-        </is>
-      </c>
-      <c r="G5" s="8" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
-      </c>
-      <c r="H5" s="9">
-        <f>F5-G5</f>
-        <v/>
-      </c>
-      <c r="I5" s="7" t="inlineStr">
-        <is>
-          <t>Nein</t>
-        </is>
-      </c>
-      <c r="J5" s="7" t="inlineStr"/>
-      <c r="K5" s="7" t="inlineStr"/>
+          <t>1. Bilanzdaten</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Bilanzpositionen für alle Unternehmen (HGB § 266) - WICHTIG: Dieses Blatt wird automatisch für Import verwendet</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="6" t="inlineStr">
         <is>
-          <t>Mutterunternehmen H</t>
-        </is>
-      </c>
-      <c r="B6" s="7" t="inlineStr">
-        <is>
-          <t>3000</t>
-        </is>
-      </c>
-      <c r="C6" s="7" t="inlineStr">
-        <is>
-          <t>Gezeichnetes Kapital</t>
-        </is>
-      </c>
-      <c r="D6" s="7" t="inlineStr">
-        <is>
-          <t>A.I</t>
-        </is>
-      </c>
-      <c r="E6" s="7" t="inlineStr">
-        <is>
-          <t>equity</t>
-        </is>
-      </c>
-      <c r="F6" s="8" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
-      </c>
-      <c r="G6" s="8" t="inlineStr">
-        <is>
-          <t>1000000.00</t>
-        </is>
-      </c>
-      <c r="H6" s="9">
-        <f>F6-G6</f>
-        <v/>
-      </c>
-      <c r="I6" s="7" t="inlineStr">
-        <is>
-          <t>Nein</t>
-        </is>
-      </c>
-      <c r="J6" s="7" t="inlineStr"/>
-      <c r="K6" s="7" t="inlineStr"/>
+          <t>2. Anleitung</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Dieses Blatt - Übersicht und Anleitung</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="6" t="inlineStr">
         <is>
-          <t>Mutterunternehmen H</t>
-        </is>
-      </c>
-      <c r="B7" s="7" t="inlineStr">
-        <is>
-          <t>3100</t>
-        </is>
-      </c>
-      <c r="C7" s="7" t="inlineStr">
-        <is>
-          <t>Kapitalrücklage</t>
-        </is>
-      </c>
-      <c r="D7" s="7" t="inlineStr">
-        <is>
-          <t>A.II</t>
-        </is>
-      </c>
-      <c r="E7" s="7" t="inlineStr">
-        <is>
-          <t>equity</t>
-        </is>
-      </c>
-      <c r="F7" s="8" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
-      </c>
-      <c r="G7" s="8" t="inlineStr">
-        <is>
-          <t>200000.00</t>
-        </is>
-      </c>
-      <c r="H7" s="9">
-        <f>F7-G7</f>
-        <v/>
-      </c>
-      <c r="I7" s="7" t="inlineStr">
-        <is>
-          <t>Nein</t>
-        </is>
-      </c>
-      <c r="J7" s="7" t="inlineStr"/>
-      <c r="K7" s="7" t="inlineStr"/>
+          <t>3. GuV-Daten</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Gewinn- und Verlustrechnung (HGB § 275)</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="6" t="inlineStr">
         <is>
-          <t>Mutterunternehmen H</t>
-        </is>
-      </c>
-      <c r="B8" s="7" t="inlineStr">
-        <is>
-          <t>3200</t>
-        </is>
-      </c>
-      <c r="C8" s="7" t="inlineStr">
-        <is>
-          <t>Gewinnrücklagen</t>
-        </is>
-      </c>
-      <c r="D8" s="7" t="inlineStr">
-        <is>
-          <t>A.III</t>
-        </is>
-      </c>
-      <c r="E8" s="7" t="inlineStr">
-        <is>
-          <t>equity</t>
-        </is>
-      </c>
-      <c r="F8" s="8" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
-      </c>
-      <c r="G8" s="8" t="inlineStr">
-        <is>
-          <t>300000.00</t>
-        </is>
-      </c>
-      <c r="H8" s="9">
-        <f>F8-G8</f>
-        <v/>
-      </c>
-      <c r="I8" s="7" t="inlineStr">
-        <is>
-          <t>Nein</t>
-        </is>
-      </c>
-      <c r="J8" s="7" t="inlineStr"/>
-      <c r="K8" s="7" t="inlineStr"/>
+          <t>4. Unternehmensinformationen</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Basis-Informationen zu allen Unternehmen</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="6" t="inlineStr">
         <is>
-          <t>Mutterunternehmen H</t>
-        </is>
-      </c>
-      <c r="B9" s="7" t="inlineStr">
-        <is>
-          <t>4000</t>
-        </is>
-      </c>
-      <c r="C9" s="7" t="inlineStr">
-        <is>
-          <t>Verbindlichkeiten</t>
-        </is>
-      </c>
-      <c r="D9" s="7" t="inlineStr">
-        <is>
-          <t>C</t>
-        </is>
-      </c>
-      <c r="E9" s="7" t="inlineStr">
-        <is>
-          <t>liability</t>
-        </is>
-      </c>
-      <c r="F9" s="8" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
-      </c>
-      <c r="G9" s="8" t="inlineStr">
-        <is>
-          <t>500000.00</t>
-        </is>
-      </c>
-      <c r="H9" s="9">
-        <f>F9-G9</f>
-        <v/>
-      </c>
-      <c r="I9" s="7" t="inlineStr">
-        <is>
-          <t>Nein</t>
-        </is>
-      </c>
-      <c r="J9" s="7" t="inlineStr"/>
-      <c r="K9" s="7" t="inlineStr"/>
+          <t>5. Beteiligungsverhältnisse</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Für Kapitalkonsolidierung (HGB § 301)</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="6" t="inlineStr">
         <is>
-          <t>Tochterunternehmen TU1</t>
-        </is>
-      </c>
-      <c r="B10" s="7" t="inlineStr">
-        <is>
-          <t>1000</t>
-        </is>
-      </c>
-      <c r="C10" s="7" t="inlineStr">
-        <is>
-          <t>Kasse</t>
-        </is>
-      </c>
-      <c r="D10" s="7" t="inlineStr">
-        <is>
-          <t>B.IV</t>
-        </is>
-      </c>
-      <c r="E10" s="7" t="inlineStr">
-        <is>
-          <t>asset</t>
-        </is>
-      </c>
-      <c r="F10" s="8" t="inlineStr">
-        <is>
-          <t>2000.00</t>
-        </is>
-      </c>
-      <c r="G10" s="8" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
-      </c>
-      <c r="H10" s="9">
-        <f>F10-G10</f>
-        <v/>
-      </c>
-      <c r="I10" s="7" t="inlineStr">
-        <is>
-          <t>Nein</t>
-        </is>
-      </c>
-      <c r="J10" s="7" t="inlineStr"/>
-      <c r="K10" s="7" t="inlineStr"/>
+          <t>6. Zwischengesellschaftsgeschäfte</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Für Schulden- und Zwischenergebniseliminierung (HGB § 303, § 305)</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="6" t="inlineStr">
         <is>
-          <t>Tochterunternehmen TU1</t>
-        </is>
-      </c>
-      <c r="B11" s="7" t="inlineStr">
-        <is>
-          <t>1600</t>
-        </is>
-      </c>
-      <c r="C11" s="7" t="inlineStr">
-        <is>
-          <t>Verbindlichkeiten a. LL</t>
-        </is>
-      </c>
-      <c r="D11" s="7" t="inlineStr">
-        <is>
-          <t>C</t>
-        </is>
-      </c>
-      <c r="E11" s="7" t="inlineStr">
-        <is>
-          <t>liability</t>
-        </is>
-      </c>
-      <c r="F11" s="8" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
-      </c>
-      <c r="G11" s="8" t="inlineStr">
-        <is>
-          <t>50000.00</t>
-        </is>
-      </c>
-      <c r="H11" s="9">
-        <f>F11-G11</f>
-        <v/>
-      </c>
-      <c r="I11" s="7" t="inlineStr">
-        <is>
-          <t>Ja</t>
-        </is>
-      </c>
-      <c r="J11" s="7" t="inlineStr">
-        <is>
-          <t>Mutter H</t>
-        </is>
-      </c>
-      <c r="K11" s="7" t="inlineStr">
-        <is>
-          <t>Gegenpartei: Mutterunternehmen H</t>
+          <t>7. Eigenkapital-Aufteilung</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Für Minderheitsanteile</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="6" t="inlineStr">
         <is>
-          <t>Tochterunternehmen TU1</t>
-        </is>
-      </c>
-      <c r="B12" s="7" t="inlineStr">
-        <is>
-          <t>3000</t>
-        </is>
-      </c>
-      <c r="C12" s="7" t="inlineStr">
-        <is>
-          <t>Gezeichnetes Kapital</t>
-        </is>
-      </c>
-      <c r="D12" s="7" t="inlineStr">
-        <is>
-          <t>A.I</t>
-        </is>
-      </c>
-      <c r="E12" s="7" t="inlineStr">
-        <is>
-          <t>equity</t>
-        </is>
-      </c>
-      <c r="F12" s="8" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
-      </c>
-      <c r="G12" s="8" t="inlineStr">
-        <is>
-          <t>500000.00</t>
-        </is>
-      </c>
-      <c r="H12" s="9">
-        <f>F12-G12</f>
-        <v/>
-      </c>
-      <c r="I12" s="7" t="inlineStr">
-        <is>
-          <t>Nein</t>
-        </is>
-      </c>
-      <c r="J12" s="7" t="inlineStr"/>
-      <c r="K12" s="7" t="inlineStr"/>
+          <t>8. Währungsumrechnung</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Für ausländische Tochterunternehmen (HGB § 256a) - NEU</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="6" t="inlineStr">
         <is>
-          <t>Tochterunternehmen TU2</t>
-        </is>
-      </c>
-      <c r="B13" s="7" t="inlineStr">
-        <is>
-          <t>1000</t>
-        </is>
-      </c>
-      <c r="C13" s="7" t="inlineStr">
-        <is>
-          <t>Kasse</t>
-        </is>
-      </c>
-      <c r="D13" s="7" t="inlineStr">
-        <is>
-          <t>B.IV</t>
-        </is>
-      </c>
-      <c r="E13" s="7" t="inlineStr">
-        <is>
-          <t>asset</t>
-        </is>
-      </c>
-      <c r="F13" s="8" t="inlineStr">
-        <is>
-          <t>1500.00</t>
-        </is>
-      </c>
-      <c r="G13" s="8" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
-      </c>
-      <c r="H13" s="9">
-        <f>F13-G13</f>
-        <v/>
-      </c>
-      <c r="I13" s="7" t="inlineStr">
-        <is>
-          <t>Nein</t>
-        </is>
-      </c>
-      <c r="J13" s="7" t="inlineStr"/>
-      <c r="K13" s="7" t="inlineStr"/>
+          <t>9. Latente Steuern</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Aktive und passive latente Steuern (HGB § 274) - NEU</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="6" t="inlineStr">
         <is>
-          <t>Tochterunternehmen TU2</t>
-        </is>
-      </c>
-      <c r="B14" s="7" t="inlineStr">
-        <is>
-          <t>3000</t>
-        </is>
-      </c>
-      <c r="C14" s="7" t="inlineStr">
-        <is>
-          <t>Gezeichnetes Kapital</t>
-        </is>
-      </c>
-      <c r="D14" s="7" t="inlineStr">
-        <is>
-          <t>A.I</t>
-        </is>
-      </c>
-      <c r="E14" s="7" t="inlineStr">
-        <is>
-          <t>equity</t>
-        </is>
-      </c>
-      <c r="F14" s="8" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
-      </c>
-      <c r="G14" s="8" t="inlineStr">
-        <is>
-          <t>300000.00</t>
-        </is>
-      </c>
-      <c r="H14" s="9">
-        <f>F14-G14</f>
-        <v/>
-      </c>
-      <c r="I14" s="7" t="inlineStr">
-        <is>
-          <t>Nein</t>
-        </is>
-      </c>
-      <c r="J14" s="7" t="inlineStr"/>
-      <c r="K14" s="7" t="inlineStr"/>
-    </row>
-    <row r="16">
-      <c r="A16" s="4" t="inlineStr">
-        <is>
-          <t>BILANZSUMME</t>
-        </is>
-      </c>
-      <c r="H16" s="10">
-        <f>SUM(H2:H14)</f>
-        <v/>
+          <t>10. HGB-Bilanzstruktur</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Referenz zur HGB-Bilanzgliederung (HGB § 266)</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="6" t="inlineStr">
+        <is>
+          <t>11. Kontenplan-Referenz</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Typische Kontonummern-Bereiche</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="10" t="inlineStr">
+        <is>
+          <t>SCHRITT-FÜR-SCHRITT-ANLEITUNG:</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="6" t="inlineStr">
+        <is>
+          <t>Schritt 1:</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Füllen Sie 'Unternehmensinformationen' aus</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="6" t="inlineStr">
+        <is>
+          <t>Schritt 2:</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Füllen Sie 'Bilanzdaten' für alle Unternehmen aus</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="6" t="inlineStr">
+        <is>
+          <t>Schritt 3:</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Füllen Sie 'GuV-Daten' für alle Unternehmen aus</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="6" t="inlineStr">
+        <is>
+          <t>Schritt 4:</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Definieren Sie 'Beteiligungsverhältnisse'</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="6" t="inlineStr">
+        <is>
+          <t>Schritt 5:</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Erfassen Sie alle 'Zwischengesellschaftsgeschäfte'</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="6" t="inlineStr">
+        <is>
+          <t>Schritt 6:</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Prüfen Sie 'Eigenkapital-Aufteilung'</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="6" t="inlineStr">
+        <is>
+          <t>Schritt 7:</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Bei ausländischen Unternehmen: 'Währungsumrechnung' ausfüllen</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="6" t="inlineStr">
+        <is>
+          <t>Schritt 8:</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>Bei Steuerdifferenzen: 'Latente Steuern' ausfüllen</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="6" t="inlineStr">
+        <is>
+          <t>Schritt 9:</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>Importieren Sie die Datei im System</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="10" t="inlineStr">
+        <is>
+          <t>HGB-REFERENZEN:</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="6" t="inlineStr">
+        <is>
+          <t>§ 266 HGB</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>Bilanzgliederung</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="6" t="inlineStr">
+        <is>
+          <t>§ 275 HGB</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>Gewinn- und Verlustrechnung</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="6" t="inlineStr">
+        <is>
+          <t>§ 301 HGB</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>Kapitalkonsolidierung</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="6" t="inlineStr">
+        <is>
+          <t>§ 303 HGB</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>Schuldenkonsolidierung</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="6" t="inlineStr">
+        <is>
+          <t>§ 305 HGB</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>Zwischenergebniseliminierung</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="6" t="inlineStr">
+        <is>
+          <t>§ 274 HGB</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>Latente Steuern</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="6" t="inlineStr">
+        <is>
+          <t>§ 256a HGB</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>Währungsumrechnung</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="10" t="inlineStr">
+        <is>
+          <t>FARBCODierung:</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="6" t="inlineStr">
+        <is>
+          <t>Blau</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>Pflichtfelder (müssen ausgefüllt werden)</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="6" t="inlineStr">
+        <is>
+          <t>Gelb</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>Optionale Felder</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="6" t="inlineStr">
+        <is>
+          <t>Grün</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>Berechnete Felder (Formeln)</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="6" t="inlineStr">
+        <is>
+          <t>Rot</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>Warnungen/Hinweise</t>
+        </is>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="26">
-    <dataValidation sqref="E2" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
-      <formula1>"asset,liability,equity"</formula1>
-    </dataValidation>
-    <dataValidation sqref="I2" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
-      <formula1>"Ja,Nein"</formula1>
-    </dataValidation>
-    <dataValidation sqref="E3" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
-      <formula1>"asset,liability,equity"</formula1>
-    </dataValidation>
-    <dataValidation sqref="I3" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
-      <formula1>"Ja,Nein"</formula1>
-    </dataValidation>
-    <dataValidation sqref="E4" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
-      <formula1>"asset,liability,equity"</formula1>
-    </dataValidation>
-    <dataValidation sqref="I4" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
-      <formula1>"Ja,Nein"</formula1>
-    </dataValidation>
-    <dataValidation sqref="E5" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
-      <formula1>"asset,liability,equity"</formula1>
-    </dataValidation>
-    <dataValidation sqref="I5" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
-      <formula1>"Ja,Nein"</formula1>
-    </dataValidation>
-    <dataValidation sqref="E6" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
-      <formula1>"asset,liability,equity"</formula1>
-    </dataValidation>
-    <dataValidation sqref="I6" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
-      <formula1>"Ja,Nein"</formula1>
-    </dataValidation>
-    <dataValidation sqref="E7" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
-      <formula1>"asset,liability,equity"</formula1>
-    </dataValidation>
-    <dataValidation sqref="I7" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
-      <formula1>"Ja,Nein"</formula1>
-    </dataValidation>
-    <dataValidation sqref="E8" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
-      <formula1>"asset,liability,equity"</formula1>
-    </dataValidation>
-    <dataValidation sqref="I8" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
-      <formula1>"Ja,Nein"</formula1>
-    </dataValidation>
-    <dataValidation sqref="E9" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
-      <formula1>"asset,liability,equity"</formula1>
-    </dataValidation>
-    <dataValidation sqref="I9" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
-      <formula1>"Ja,Nein"</formula1>
-    </dataValidation>
-    <dataValidation sqref="E10" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
-      <formula1>"asset,liability,equity"</formula1>
-    </dataValidation>
-    <dataValidation sqref="I10" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
-      <formula1>"Ja,Nein"</formula1>
-    </dataValidation>
-    <dataValidation sqref="E11" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
-      <formula1>"asset,liability,equity"</formula1>
-    </dataValidation>
-    <dataValidation sqref="I11" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
-      <formula1>"Ja,Nein"</formula1>
-    </dataValidation>
-    <dataValidation sqref="E12" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
-      <formula1>"asset,liability,equity"</formula1>
-    </dataValidation>
-    <dataValidation sqref="I12" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
-      <formula1>"Ja,Nein"</formula1>
-    </dataValidation>
-    <dataValidation sqref="E13" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
-      <formula1>"asset,liability,equity"</formula1>
-    </dataValidation>
-    <dataValidation sqref="I13" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
-      <formula1>"Ja,Nein"</formula1>
-    </dataValidation>
-    <dataValidation sqref="E14" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
-      <formula1>"asset,liability,equity"</formula1>
-    </dataValidation>
-    <dataValidation sqref="I14" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
-      <formula1>"Ja,Nein"</formula1>
-    </dataValidation>
-  </dataValidations>
+  <mergeCells count="2">
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="A1:F1"/>
+  </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -2369,470 +2388,470 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="5" t="inlineStr">
+      <c r="A1" s="1" t="inlineStr">
         <is>
           <t>Unternehmen</t>
         </is>
       </c>
-      <c r="B1" s="5" t="inlineStr">
+      <c r="B1" s="1" t="inlineStr">
         <is>
           <t>Kontonummer</t>
         </is>
       </c>
-      <c r="C1" s="5" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>Kontoname</t>
         </is>
       </c>
-      <c r="D1" s="5" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>Kontotyp</t>
         </is>
       </c>
-      <c r="E1" s="5" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>Betrag</t>
         </is>
       </c>
-      <c r="F1" s="5" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>Zwischengesellschaft</t>
         </is>
       </c>
-      <c r="G1" s="5" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>Gegenpartei</t>
         </is>
       </c>
-      <c r="H1" s="5" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>Bemerkung</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="6" t="inlineStr">
+      <c r="A2" s="2" t="inlineStr">
         <is>
           <t>Mutterunternehmen H</t>
         </is>
       </c>
-      <c r="B2" s="7" t="inlineStr">
+      <c r="B2" s="3" t="inlineStr">
         <is>
           <t>8000</t>
         </is>
       </c>
-      <c r="C2" s="7" t="inlineStr">
+      <c r="C2" s="3" t="inlineStr">
         <is>
           <t>Umsatzerlöse</t>
         </is>
       </c>
-      <c r="D2" s="7" t="inlineStr">
+      <c r="D2" s="3" t="inlineStr">
         <is>
           <t>revenue</t>
         </is>
       </c>
-      <c r="E2" s="8" t="inlineStr">
+      <c r="E2" s="4" t="inlineStr">
         <is>
           <t>1000000.00</t>
         </is>
       </c>
-      <c r="F2" s="7" t="inlineStr">
+      <c r="F2" s="3" t="inlineStr">
         <is>
           <t>Nein</t>
         </is>
       </c>
-      <c r="G2" s="7" t="inlineStr"/>
-      <c r="H2" s="7" t="inlineStr"/>
+      <c r="G2" s="3" t="inlineStr"/>
+      <c r="H2" s="3" t="inlineStr"/>
     </row>
     <row r="3">
-      <c r="A3" s="6" t="inlineStr">
+      <c r="A3" s="2" t="inlineStr">
         <is>
           <t>Mutterunternehmen H</t>
         </is>
       </c>
-      <c r="B3" s="7" t="inlineStr">
+      <c r="B3" s="3" t="inlineStr">
         <is>
           <t>8000</t>
         </is>
       </c>
-      <c r="C3" s="7" t="inlineStr">
+      <c r="C3" s="3" t="inlineStr">
         <is>
           <t>Umsatzerlöse (an TU1)</t>
         </is>
       </c>
-      <c r="D3" s="7" t="inlineStr">
+      <c r="D3" s="3" t="inlineStr">
         <is>
           <t>revenue</t>
         </is>
       </c>
-      <c r="E3" s="8" t="inlineStr">
+      <c r="E3" s="4" t="inlineStr">
         <is>
           <t>100000.00</t>
         </is>
       </c>
-      <c r="F3" s="7" t="inlineStr">
+      <c r="F3" s="3" t="inlineStr">
         <is>
           <t>Ja</t>
         </is>
       </c>
-      <c r="G3" s="7" t="inlineStr">
+      <c r="G3" s="3" t="inlineStr">
         <is>
           <t>TU1</t>
         </is>
       </c>
-      <c r="H3" s="7" t="inlineStr">
+      <c r="H3" s="3" t="inlineStr">
         <is>
           <t>Zwischenumsatz</t>
         </is>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="6" t="inlineStr">
+      <c r="A4" s="2" t="inlineStr">
         <is>
           <t>Mutterunternehmen H</t>
         </is>
       </c>
-      <c r="B4" s="7" t="inlineStr">
+      <c r="B4" s="3" t="inlineStr">
         <is>
           <t>4000</t>
         </is>
       </c>
-      <c r="C4" s="7" t="inlineStr">
+      <c r="C4" s="3" t="inlineStr">
         <is>
           <t>Materialaufwand</t>
         </is>
       </c>
-      <c r="D4" s="7" t="inlineStr">
+      <c r="D4" s="3" t="inlineStr">
         <is>
           <t>cost_of_sales</t>
         </is>
       </c>
-      <c r="E4" s="8" t="inlineStr">
+      <c r="E4" s="4" t="inlineStr">
         <is>
           <t>600000.00</t>
         </is>
       </c>
-      <c r="F4" s="7" t="inlineStr">
+      <c r="F4" s="3" t="inlineStr">
         <is>
           <t>Nein</t>
         </is>
       </c>
-      <c r="G4" s="7" t="inlineStr"/>
-      <c r="H4" s="7" t="inlineStr"/>
+      <c r="G4" s="3" t="inlineStr"/>
+      <c r="H4" s="3" t="inlineStr"/>
     </row>
     <row r="5">
-      <c r="A5" s="6" t="inlineStr">
+      <c r="A5" s="2" t="inlineStr">
         <is>
           <t>Mutterunternehmen H</t>
         </is>
       </c>
-      <c r="B5" s="7" t="inlineStr">
+      <c r="B5" s="3" t="inlineStr">
         <is>
           <t>6000</t>
         </is>
       </c>
-      <c r="C5" s="7" t="inlineStr">
+      <c r="C5" s="3" t="inlineStr">
         <is>
           <t>Personalaufwand</t>
         </is>
       </c>
-      <c r="D5" s="7" t="inlineStr">
+      <c r="D5" s="3" t="inlineStr">
         <is>
           <t>operating_expense</t>
         </is>
       </c>
-      <c r="E5" s="8" t="inlineStr">
+      <c r="E5" s="4" t="inlineStr">
         <is>
           <t>200000.00</t>
         </is>
       </c>
-      <c r="F5" s="7" t="inlineStr">
+      <c r="F5" s="3" t="inlineStr">
         <is>
           <t>Nein</t>
         </is>
       </c>
-      <c r="G5" s="7" t="inlineStr"/>
-      <c r="H5" s="7" t="inlineStr"/>
+      <c r="G5" s="3" t="inlineStr"/>
+      <c r="H5" s="3" t="inlineStr"/>
     </row>
     <row r="6">
-      <c r="A6" s="6" t="inlineStr">
+      <c r="A6" s="2" t="inlineStr">
         <is>
           <t>Mutterunternehmen H</t>
         </is>
       </c>
-      <c r="B6" s="7" t="inlineStr">
+      <c r="B6" s="3" t="inlineStr">
         <is>
           <t>7000</t>
         </is>
       </c>
-      <c r="C6" s="7" t="inlineStr">
+      <c r="C6" s="3" t="inlineStr">
         <is>
           <t>Abschreibungen</t>
         </is>
       </c>
-      <c r="D6" s="7" t="inlineStr">
+      <c r="D6" s="3" t="inlineStr">
         <is>
           <t>operating_expense</t>
         </is>
       </c>
-      <c r="E6" s="8" t="inlineStr">
+      <c r="E6" s="4" t="inlineStr">
         <is>
           <t>50000.00</t>
         </is>
       </c>
-      <c r="F6" s="7" t="inlineStr">
+      <c r="F6" s="3" t="inlineStr">
         <is>
           <t>Nein</t>
         </is>
       </c>
-      <c r="G6" s="7" t="inlineStr"/>
-      <c r="H6" s="7" t="inlineStr"/>
+      <c r="G6" s="3" t="inlineStr"/>
+      <c r="H6" s="3" t="inlineStr"/>
     </row>
     <row r="7">
-      <c r="A7" s="6" t="inlineStr">
+      <c r="A7" s="2" t="inlineStr">
         <is>
           <t>Mutterunternehmen H</t>
         </is>
       </c>
-      <c r="B7" s="7" t="inlineStr">
+      <c r="B7" s="3" t="inlineStr">
         <is>
           <t>7500</t>
         </is>
       </c>
-      <c r="C7" s="7" t="inlineStr">
+      <c r="C7" s="3" t="inlineStr">
         <is>
           <t>Zinsaufwand</t>
         </is>
       </c>
-      <c r="D7" s="7" t="inlineStr">
+      <c r="D7" s="3" t="inlineStr">
         <is>
           <t>financial_expense</t>
         </is>
       </c>
-      <c r="E7" s="8" t="inlineStr">
+      <c r="E7" s="4" t="inlineStr">
         <is>
           <t>10000.00</t>
         </is>
       </c>
-      <c r="F7" s="7" t="inlineStr">
+      <c r="F7" s="3" t="inlineStr">
         <is>
           <t>Nein</t>
         </is>
       </c>
-      <c r="G7" s="7" t="inlineStr"/>
-      <c r="H7" s="7" t="inlineStr"/>
+      <c r="G7" s="3" t="inlineStr"/>
+      <c r="H7" s="3" t="inlineStr"/>
     </row>
     <row r="8">
-      <c r="A8" s="6" t="inlineStr">
+      <c r="A8" s="2" t="inlineStr">
         <is>
           <t>Tochterunternehmen TU1</t>
         </is>
       </c>
-      <c r="B8" s="7" t="inlineStr">
+      <c r="B8" s="3" t="inlineStr">
         <is>
           <t>8000</t>
         </is>
       </c>
-      <c r="C8" s="7" t="inlineStr">
+      <c r="C8" s="3" t="inlineStr">
         <is>
           <t>Umsatzerlöse</t>
         </is>
       </c>
-      <c r="D8" s="7" t="inlineStr">
+      <c r="D8" s="3" t="inlineStr">
         <is>
           <t>revenue</t>
         </is>
       </c>
-      <c r="E8" s="8" t="inlineStr">
+      <c r="E8" s="4" t="inlineStr">
         <is>
           <t>500000.00</t>
         </is>
       </c>
-      <c r="F8" s="7" t="inlineStr">
+      <c r="F8" s="3" t="inlineStr">
         <is>
           <t>Nein</t>
         </is>
       </c>
-      <c r="G8" s="7" t="inlineStr"/>
-      <c r="H8" s="7" t="inlineStr"/>
+      <c r="G8" s="3" t="inlineStr"/>
+      <c r="H8" s="3" t="inlineStr"/>
     </row>
     <row r="9">
-      <c r="A9" s="6" t="inlineStr">
+      <c r="A9" s="2" t="inlineStr">
         <is>
           <t>Tochterunternehmen TU1</t>
         </is>
       </c>
-      <c r="B9" s="7" t="inlineStr">
+      <c r="B9" s="3" t="inlineStr">
         <is>
           <t>4000</t>
         </is>
       </c>
-      <c r="C9" s="7" t="inlineStr">
+      <c r="C9" s="3" t="inlineStr">
         <is>
           <t>Materialaufwand</t>
         </is>
       </c>
-      <c r="D9" s="7" t="inlineStr">
+      <c r="D9" s="3" t="inlineStr">
         <is>
           <t>cost_of_sales</t>
         </is>
       </c>
-      <c r="E9" s="8" t="inlineStr">
+      <c r="E9" s="4" t="inlineStr">
         <is>
           <t>300000.00</t>
         </is>
       </c>
-      <c r="F9" s="7" t="inlineStr">
+      <c r="F9" s="3" t="inlineStr">
         <is>
           <t>Nein</t>
         </is>
       </c>
-      <c r="G9" s="7" t="inlineStr"/>
-      <c r="H9" s="7" t="inlineStr"/>
+      <c r="G9" s="3" t="inlineStr"/>
+      <c r="H9" s="3" t="inlineStr"/>
     </row>
     <row r="10">
-      <c r="A10" s="6" t="inlineStr">
+      <c r="A10" s="2" t="inlineStr">
         <is>
           <t>Tochterunternehmen TU1</t>
         </is>
       </c>
-      <c r="B10" s="7" t="inlineStr">
+      <c r="B10" s="3" t="inlineStr">
         <is>
           <t>4000</t>
         </is>
       </c>
-      <c r="C10" s="7" t="inlineStr">
+      <c r="C10" s="3" t="inlineStr">
         <is>
           <t>Materialaufwand (von Mutter H)</t>
         </is>
       </c>
-      <c r="D10" s="7" t="inlineStr">
+      <c r="D10" s="3" t="inlineStr">
         <is>
           <t>cost_of_sales</t>
         </is>
       </c>
-      <c r="E10" s="8" t="inlineStr">
+      <c r="E10" s="4" t="inlineStr">
         <is>
           <t>80000.00</t>
         </is>
       </c>
-      <c r="F10" s="7" t="inlineStr">
+      <c r="F10" s="3" t="inlineStr">
         <is>
           <t>Ja</t>
         </is>
       </c>
-      <c r="G10" s="7" t="inlineStr">
+      <c r="G10" s="3" t="inlineStr">
         <is>
           <t>Mutter H</t>
         </is>
       </c>
-      <c r="H10" s="7" t="inlineStr">
+      <c r="H10" s="3" t="inlineStr">
         <is>
           <t>Zwischenaufwand</t>
         </is>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="6" t="inlineStr">
+      <c r="A11" s="2" t="inlineStr">
         <is>
           <t>Tochterunternehmen TU1</t>
         </is>
       </c>
-      <c r="B11" s="7" t="inlineStr">
+      <c r="B11" s="3" t="inlineStr">
         <is>
           <t>6000</t>
         </is>
       </c>
-      <c r="C11" s="7" t="inlineStr">
+      <c r="C11" s="3" t="inlineStr">
         <is>
           <t>Personalaufwand</t>
         </is>
       </c>
-      <c r="D11" s="7" t="inlineStr">
+      <c r="D11" s="3" t="inlineStr">
         <is>
           <t>operating_expense</t>
         </is>
       </c>
-      <c r="E11" s="8" t="inlineStr">
+      <c r="E11" s="4" t="inlineStr">
         <is>
           <t>100000.00</t>
         </is>
       </c>
-      <c r="F11" s="7" t="inlineStr">
+      <c r="F11" s="3" t="inlineStr">
         <is>
           <t>Nein</t>
         </is>
       </c>
-      <c r="G11" s="7" t="inlineStr"/>
-      <c r="H11" s="7" t="inlineStr"/>
+      <c r="G11" s="3" t="inlineStr"/>
+      <c r="H11" s="3" t="inlineStr"/>
     </row>
     <row r="12">
-      <c r="A12" s="6" t="inlineStr">
+      <c r="A12" s="2" t="inlineStr">
         <is>
           <t>Tochterunternehmen TU2</t>
         </is>
       </c>
-      <c r="B12" s="7" t="inlineStr">
+      <c r="B12" s="3" t="inlineStr">
         <is>
           <t>8000</t>
         </is>
       </c>
-      <c r="C12" s="7" t="inlineStr">
+      <c r="C12" s="3" t="inlineStr">
         <is>
           <t>Umsatzerlöse</t>
         </is>
       </c>
-      <c r="D12" s="7" t="inlineStr">
+      <c r="D12" s="3" t="inlineStr">
         <is>
           <t>revenue</t>
         </is>
       </c>
-      <c r="E12" s="8" t="inlineStr">
+      <c r="E12" s="4" t="inlineStr">
         <is>
           <t>200000.00</t>
         </is>
       </c>
-      <c r="F12" s="7" t="inlineStr">
+      <c r="F12" s="3" t="inlineStr">
         <is>
           <t>Nein</t>
         </is>
       </c>
-      <c r="G12" s="7" t="inlineStr"/>
-      <c r="H12" s="7" t="inlineStr"/>
+      <c r="G12" s="3" t="inlineStr"/>
+      <c r="H12" s="3" t="inlineStr"/>
     </row>
     <row r="13">
-      <c r="A13" s="6" t="inlineStr">
+      <c r="A13" s="2" t="inlineStr">
         <is>
           <t>Tochterunternehmen TU2</t>
         </is>
       </c>
-      <c r="B13" s="7" t="inlineStr">
+      <c r="B13" s="3" t="inlineStr">
         <is>
           <t>4000</t>
         </is>
       </c>
-      <c r="C13" s="7" t="inlineStr">
+      <c r="C13" s="3" t="inlineStr">
         <is>
           <t>Materialaufwand</t>
         </is>
       </c>
-      <c r="D13" s="7" t="inlineStr">
+      <c r="D13" s="3" t="inlineStr">
         <is>
           <t>cost_of_sales</t>
         </is>
       </c>
-      <c r="E13" s="8" t="inlineStr">
+      <c r="E13" s="4" t="inlineStr">
         <is>
           <t>120000.00</t>
         </is>
       </c>
-      <c r="F13" s="7" t="inlineStr">
+      <c r="F13" s="3" t="inlineStr">
         <is>
           <t>Nein</t>
         </is>
       </c>
-      <c r="G13" s="7" t="inlineStr"/>
-      <c r="H13" s="7" t="inlineStr"/>
+      <c r="G13" s="3" t="inlineStr"/>
+      <c r="H13" s="3" t="inlineStr"/>
     </row>
   </sheetData>
   <dataValidations count="24">
@@ -2936,44 +2955,44 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="5" t="inlineStr">
+      <c r="A1" s="1" t="inlineStr">
         <is>
           <t>Unternehmensname</t>
         </is>
       </c>
-      <c r="B1" s="5" t="inlineStr">
+      <c r="B1" s="1" t="inlineStr">
         <is>
           <t>Typ</t>
         </is>
       </c>
-      <c r="C1" s="5" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>Beteiligungs-%</t>
         </is>
       </c>
-      <c r="D1" s="5" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>Erwerbsdatum</t>
         </is>
       </c>
-      <c r="E1" s="5" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>Anschaffungskosten</t>
         </is>
       </c>
-      <c r="F1" s="5" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>Bemerkung</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="6" t="inlineStr">
+      <c r="A2" s="2" t="inlineStr">
         <is>
           <t>Mutterunternehmen H</t>
         </is>
       </c>
-      <c r="B2" s="7" t="inlineStr">
+      <c r="B2" s="3" t="inlineStr">
         <is>
           <t>Mutterunternehmen (H)</t>
         </is>
@@ -2983,21 +3002,21 @@
           <t>100.00</t>
         </is>
       </c>
-      <c r="D2" s="7" t="inlineStr"/>
+      <c r="D2" s="3" t="inlineStr"/>
       <c r="E2" s="12" t="inlineStr"/>
-      <c r="F2" s="7" t="inlineStr">
+      <c r="F2" s="3" t="inlineStr">
         <is>
           <t>Hauptunternehmen</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="6" t="inlineStr">
+      <c r="A3" s="2" t="inlineStr">
         <is>
           <t>Tochterunternehmen TU1</t>
         </is>
       </c>
-      <c r="B3" s="7" t="inlineStr">
+      <c r="B3" s="3" t="inlineStr">
         <is>
           <t>Tochterunternehmen (TU)</t>
         </is>
@@ -3007,7 +3026,7 @@
           <t>80.00</t>
         </is>
       </c>
-      <c r="D3" s="7" t="inlineStr">
+      <c r="D3" s="3" t="inlineStr">
         <is>
           <t>2020-01-15</t>
         </is>
@@ -3017,19 +3036,19 @@
           <t>500000.00</t>
         </is>
       </c>
-      <c r="F3" s="7" t="inlineStr">
+      <c r="F3" s="3" t="inlineStr">
         <is>
           <t>80% Beteiligung</t>
         </is>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="6" t="inlineStr">
+      <c r="A4" s="2" t="inlineStr">
         <is>
           <t>Tochterunternehmen TU2</t>
         </is>
       </c>
-      <c r="B4" s="7" t="inlineStr">
+      <c r="B4" s="3" t="inlineStr">
         <is>
           <t>Tochterunternehmen (TU)</t>
         </is>
@@ -3039,7 +3058,7 @@
           <t>60.00</t>
         </is>
       </c>
-      <c r="D4" s="7" t="inlineStr">
+      <c r="D4" s="3" t="inlineStr">
         <is>
           <t>2021-06-01</t>
         </is>
@@ -3049,7 +3068,7 @@
           <t>300000.00</t>
         </is>
       </c>
-      <c r="F4" s="7" t="inlineStr">
+      <c r="F4" s="3" t="inlineStr">
         <is>
           <t>60% Beteiligung</t>
         </is>
@@ -3084,49 +3103,49 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="5" t="inlineStr">
+      <c r="A1" s="1" t="inlineStr">
         <is>
           <t>Mutterunternehmen</t>
         </is>
       </c>
-      <c r="B1" s="5" t="inlineStr">
+      <c r="B1" s="1" t="inlineStr">
         <is>
           <t>Tochterunternehmen</t>
         </is>
       </c>
-      <c r="C1" s="5" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>Beteiligungs-%</t>
         </is>
       </c>
-      <c r="D1" s="5" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>Anschaffungskosten</t>
         </is>
       </c>
-      <c r="E1" s="5" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>Erwerbsdatum</t>
         </is>
       </c>
-      <c r="F1" s="5" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>Beteiligungsbuchwert</t>
         </is>
       </c>
-      <c r="G1" s="5" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>Bemerkung</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="7" t="inlineStr">
+      <c r="A2" s="3" t="inlineStr">
         <is>
           <t>Mutterunternehmen H</t>
         </is>
       </c>
-      <c r="B2" s="7" t="inlineStr">
+      <c r="B2" s="3" t="inlineStr">
         <is>
           <t>Tochterunternehmen TU1</t>
         </is>
@@ -3141,7 +3160,7 @@
           <t>500000.00</t>
         </is>
       </c>
-      <c r="E2" s="7" t="inlineStr">
+      <c r="E2" s="3" t="inlineStr">
         <is>
           <t>2020-01-15</t>
         </is>
@@ -3151,19 +3170,19 @@
           <t>500000.00</t>
         </is>
       </c>
-      <c r="G2" s="7" t="inlineStr">
+      <c r="G2" s="3" t="inlineStr">
         <is>
           <t>Nach HGB § 301</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="7" t="inlineStr">
+      <c r="A3" s="3" t="inlineStr">
         <is>
           <t>Mutterunternehmen H</t>
         </is>
       </c>
-      <c r="B3" s="7" t="inlineStr">
+      <c r="B3" s="3" t="inlineStr">
         <is>
           <t>Tochterunternehmen TU2</t>
         </is>
@@ -3178,7 +3197,7 @@
           <t>300000.00</t>
         </is>
       </c>
-      <c r="E3" s="7" t="inlineStr">
+      <c r="E3" s="3" t="inlineStr">
         <is>
           <t>2021-06-01</t>
         </is>
@@ -3188,7 +3207,7 @@
           <t>300000.00</t>
         </is>
       </c>
-      <c r="G3" s="7" t="inlineStr">
+      <c r="G3" s="3" t="inlineStr">
         <is>
           <t>Nach HGB § 301</t>
         </is>
@@ -3228,302 +3247,302 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="5" t="inlineStr">
+      <c r="A1" s="1" t="inlineStr">
         <is>
           <t>Transaktions-ID</t>
         </is>
       </c>
-      <c r="B1" s="5" t="inlineStr">
+      <c r="B1" s="1" t="inlineStr">
         <is>
           <t>Von Unternehmen</t>
         </is>
       </c>
-      <c r="C1" s="5" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>An Unternehmen</t>
         </is>
       </c>
-      <c r="D1" s="5" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>Transaktionstyp</t>
         </is>
       </c>
-      <c r="E1" s="5" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>Betrag</t>
         </is>
       </c>
-      <c r="F1" s="5" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>Kontonummer</t>
         </is>
       </c>
-      <c r="G1" s="5" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>Kontoname</t>
         </is>
       </c>
-      <c r="H1" s="5" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>Gewinnmarge</t>
         </is>
       </c>
-      <c r="I1" s="5" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>Eliminierungsmethode</t>
         </is>
       </c>
-      <c r="J1" s="5" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>Eliminierungsbetrag</t>
         </is>
       </c>
-      <c r="K1" s="5" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>HGB-Referenz</t>
         </is>
       </c>
-      <c r="L1" s="5" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>Bemerkung</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="7" t="inlineStr">
+      <c r="A2" s="3" t="inlineStr">
         <is>
           <t>T001</t>
         </is>
       </c>
-      <c r="B2" s="7" t="inlineStr">
+      <c r="B2" s="3" t="inlineStr">
         <is>
           <t>Mutterunternehmen H</t>
         </is>
       </c>
-      <c r="C2" s="7" t="inlineStr">
+      <c r="C2" s="3" t="inlineStr">
         <is>
           <t>Tochterunternehmen TU1</t>
         </is>
       </c>
-      <c r="D2" s="7" t="inlineStr">
+      <c r="D2" s="3" t="inlineStr">
         <is>
           <t>Forderung</t>
         </is>
       </c>
-      <c r="E2" s="8" t="inlineStr">
+      <c r="E2" s="4" t="inlineStr">
         <is>
           <t>50000.00</t>
         </is>
       </c>
-      <c r="F2" s="7" t="inlineStr">
+      <c r="F2" s="3" t="inlineStr">
         <is>
           <t>1200</t>
         </is>
       </c>
-      <c r="G2" s="7" t="inlineStr">
+      <c r="G2" s="3" t="inlineStr">
         <is>
           <t>Forderungen a. LL</t>
         </is>
       </c>
-      <c r="H2" s="8" t="inlineStr"/>
-      <c r="I2" s="7" t="inlineStr">
+      <c r="H2" s="4" t="inlineStr"/>
+      <c r="I2" s="3" t="inlineStr">
         <is>
           <t>Vollständig</t>
         </is>
       </c>
-      <c r="J2" s="8" t="inlineStr">
+      <c r="J2" s="4" t="inlineStr">
         <is>
           <t>50000.00</t>
         </is>
       </c>
-      <c r="K2" s="7" t="inlineStr">
+      <c r="K2" s="3" t="inlineStr">
         <is>
           <t>§ 303</t>
         </is>
       </c>
-      <c r="L2" s="7" t="inlineStr">
+      <c r="L2" s="3" t="inlineStr">
         <is>
           <t>Zu eliminieren</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="7" t="inlineStr">
+      <c r="A3" s="3" t="inlineStr">
         <is>
           <t>T001</t>
         </is>
       </c>
-      <c r="B3" s="7" t="inlineStr">
+      <c r="B3" s="3" t="inlineStr">
         <is>
           <t>Tochterunternehmen TU1</t>
         </is>
       </c>
-      <c r="C3" s="7" t="inlineStr">
+      <c r="C3" s="3" t="inlineStr">
         <is>
           <t>Mutterunternehmen H</t>
         </is>
       </c>
-      <c r="D3" s="7" t="inlineStr">
+      <c r="D3" s="3" t="inlineStr">
         <is>
           <t>Verbindlichkeit</t>
         </is>
       </c>
-      <c r="E3" s="8" t="inlineStr">
+      <c r="E3" s="4" t="inlineStr">
         <is>
           <t>50000.00</t>
         </is>
       </c>
-      <c r="F3" s="7" t="inlineStr">
+      <c r="F3" s="3" t="inlineStr">
         <is>
           <t>1600</t>
         </is>
       </c>
-      <c r="G3" s="7" t="inlineStr">
+      <c r="G3" s="3" t="inlineStr">
         <is>
           <t>Verbindlichkeiten a. LL</t>
         </is>
       </c>
-      <c r="H3" s="8" t="inlineStr"/>
-      <c r="I3" s="7" t="inlineStr">
+      <c r="H3" s="4" t="inlineStr"/>
+      <c r="I3" s="3" t="inlineStr">
         <is>
           <t>Vollständig</t>
         </is>
       </c>
-      <c r="J3" s="8" t="inlineStr">
+      <c r="J3" s="4" t="inlineStr">
         <is>
           <t>50000.00</t>
         </is>
       </c>
-      <c r="K3" s="7" t="inlineStr">
+      <c r="K3" s="3" t="inlineStr">
         <is>
           <t>§ 303</t>
         </is>
       </c>
-      <c r="L3" s="7" t="inlineStr">
+      <c r="L3" s="3" t="inlineStr">
         <is>
           <t>Zu eliminieren</t>
         </is>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="7" t="inlineStr">
+      <c r="A4" s="3" t="inlineStr">
         <is>
           <t>T002</t>
         </is>
       </c>
-      <c r="B4" s="7" t="inlineStr">
+      <c r="B4" s="3" t="inlineStr">
         <is>
           <t>Mutterunternehmen H</t>
         </is>
       </c>
-      <c r="C4" s="7" t="inlineStr">
+      <c r="C4" s="3" t="inlineStr">
         <is>
           <t>Tochterunternehmen TU1</t>
         </is>
       </c>
-      <c r="D4" s="7" t="inlineStr">
+      <c r="D4" s="3" t="inlineStr">
         <is>
           <t>Lieferung</t>
         </is>
       </c>
-      <c r="E4" s="8" t="inlineStr">
+      <c r="E4" s="4" t="inlineStr">
         <is>
           <t>100000.00</t>
         </is>
       </c>
-      <c r="F4" s="7" t="inlineStr">
+      <c r="F4" s="3" t="inlineStr">
         <is>
           <t>8000</t>
         </is>
       </c>
-      <c r="G4" s="7" t="inlineStr">
+      <c r="G4" s="3" t="inlineStr">
         <is>
           <t>Umsatzerlöse</t>
         </is>
       </c>
-      <c r="H4" s="8" t="inlineStr">
+      <c r="H4" s="4" t="inlineStr">
         <is>
           <t>20.00</t>
         </is>
       </c>
-      <c r="I4" s="7" t="inlineStr">
+      <c r="I4" s="3" t="inlineStr">
         <is>
           <t>Vollständig</t>
         </is>
       </c>
-      <c r="J4" s="8" t="inlineStr">
+      <c r="J4" s="4" t="inlineStr">
         <is>
           <t>20000.00</t>
         </is>
       </c>
-      <c r="K4" s="7" t="inlineStr">
+      <c r="K4" s="3" t="inlineStr">
         <is>
           <t>§ 305</t>
         </is>
       </c>
-      <c r="L4" s="7" t="inlineStr">
+      <c r="L4" s="3" t="inlineStr">
         <is>
           <t>Zwischengewinn zu eliminieren</t>
         </is>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="7" t="inlineStr">
+      <c r="A5" s="3" t="inlineStr">
         <is>
           <t>T003</t>
         </is>
       </c>
-      <c r="B5" s="7" t="inlineStr">
+      <c r="B5" s="3" t="inlineStr">
         <is>
           <t>Mutterunternehmen H</t>
         </is>
       </c>
-      <c r="C5" s="7" t="inlineStr">
+      <c r="C5" s="3" t="inlineStr">
         <is>
           <t>Tochterunternehmen TU2</t>
         </is>
       </c>
-      <c r="D5" s="7" t="inlineStr">
+      <c r="D5" s="3" t="inlineStr">
         <is>
           <t>Dienstleistung</t>
         </is>
       </c>
-      <c r="E5" s="8" t="inlineStr">
+      <c r="E5" s="4" t="inlineStr">
         <is>
           <t>30000.00</t>
         </is>
       </c>
-      <c r="F5" s="7" t="inlineStr">
+      <c r="F5" s="3" t="inlineStr">
         <is>
           <t>8000</t>
         </is>
       </c>
-      <c r="G5" s="7" t="inlineStr">
+      <c r="G5" s="3" t="inlineStr">
         <is>
           <t>Umsatzerlöse</t>
         </is>
       </c>
-      <c r="H5" s="8" t="inlineStr">
+      <c r="H5" s="4" t="inlineStr">
         <is>
           <t>15.00</t>
         </is>
       </c>
-      <c r="I5" s="7" t="inlineStr">
+      <c r="I5" s="3" t="inlineStr">
         <is>
           <t>Vollständig</t>
         </is>
       </c>
-      <c r="J5" s="8" t="inlineStr">
+      <c r="J5" s="4" t="inlineStr">
         <is>
           <t>4500.00</t>
         </is>
       </c>
-      <c r="K5" s="7" t="inlineStr">
+      <c r="K5" s="3" t="inlineStr">
         <is>
           <t>§ 305</t>
         </is>
       </c>
-      <c r="L5" s="7" t="inlineStr">
+      <c r="L5" s="3" t="inlineStr">
         <is>
           <t>Zwischengewinn zu eliminieren</t>
         </is>
@@ -3597,49 +3616,49 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="5" t="inlineStr">
+      <c r="A1" s="1" t="inlineStr">
         <is>
           <t>Unternehmen</t>
         </is>
       </c>
-      <c r="B1" s="5" t="inlineStr">
+      <c r="B1" s="1" t="inlineStr">
         <is>
           <t>Gezeichnetes Kapital</t>
         </is>
       </c>
-      <c r="C1" s="5" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>Kapitalrücklagen</t>
         </is>
       </c>
-      <c r="D1" s="5" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>Gewinnrücklagen</t>
         </is>
       </c>
-      <c r="E1" s="5" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>Jahresüberschuss</t>
         </is>
       </c>
-      <c r="F1" s="5" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>Gesamt Eigenkapital</t>
         </is>
       </c>
-      <c r="G1" s="5" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>Anteil Mutter</t>
         </is>
       </c>
-      <c r="H1" s="5" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>Anteil Minderheit</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="7" t="inlineStr">
+      <c r="A2" s="3" t="inlineStr">
         <is>
           <t>Mutterunternehmen H</t>
         </is>
@@ -3679,7 +3698,7 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="7" t="inlineStr">
+      <c r="A3" s="3" t="inlineStr">
         <is>
           <t>Tochterunternehmen TU1</t>
         </is>
@@ -3719,7 +3738,7 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="7" t="inlineStr">
+      <c r="A4" s="3" t="inlineStr">
         <is>
           <t>Tochterunternehmen TU2</t>
         </is>
@@ -3793,44 +3812,44 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="5" t="inlineStr">
+      <c r="A2" s="1" t="inlineStr">
         <is>
           <t>Unternehmen</t>
         </is>
       </c>
-      <c r="B2" s="5" t="inlineStr">
+      <c r="B2" s="1" t="inlineStr">
         <is>
           <t>Währung (ISO)</t>
         </is>
       </c>
-      <c r="C2" s="5" t="inlineStr">
+      <c r="C2" s="1" t="inlineStr">
         <is>
           <t>Umrechnungskurs (Stichtag)</t>
         </is>
       </c>
-      <c r="D2" s="5" t="inlineStr">
+      <c r="D2" s="1" t="inlineStr">
         <is>
           <t>Durchschnittskurs (GuV)</t>
         </is>
       </c>
-      <c r="E2" s="5" t="inlineStr">
+      <c r="E2" s="1" t="inlineStr">
         <is>
           <t>Umrechnungsdatum</t>
         </is>
       </c>
-      <c r="F2" s="5" t="inlineStr">
+      <c r="F2" s="1" t="inlineStr">
         <is>
           <t>Bemerkung</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="6" t="inlineStr">
+      <c r="A3" s="2" t="inlineStr">
         <is>
           <t>Mutterunternehmen H</t>
         </is>
       </c>
-      <c r="B3" s="7" t="inlineStr">
+      <c r="B3" s="3" t="inlineStr">
         <is>
           <t>EUR</t>
         </is>
@@ -3845,24 +3864,24 @@
           <t>1.0000</t>
         </is>
       </c>
-      <c r="E3" s="7" t="inlineStr">
+      <c r="E3" s="3" t="inlineStr">
         <is>
           <t>2024-12-31</t>
         </is>
       </c>
-      <c r="F3" s="7" t="inlineStr">
+      <c r="F3" s="3" t="inlineStr">
         <is>
           <t>Hauptwährung</t>
         </is>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="6" t="inlineStr">
+      <c r="A4" s="2" t="inlineStr">
         <is>
           <t>Tochterunternehmen TU1</t>
         </is>
       </c>
-      <c r="B4" s="7" t="inlineStr">
+      <c r="B4" s="3" t="inlineStr">
         <is>
           <t>EUR</t>
         </is>
@@ -3877,24 +3896,24 @@
           <t>1.0000</t>
         </is>
       </c>
-      <c r="E4" s="7" t="inlineStr">
+      <c r="E4" s="3" t="inlineStr">
         <is>
           <t>2024-12-31</t>
         </is>
       </c>
-      <c r="F4" s="7" t="inlineStr">
+      <c r="F4" s="3" t="inlineStr">
         <is>
           <t>Gleiche Währung</t>
         </is>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="6" t="inlineStr">
+      <c r="A5" s="2" t="inlineStr">
         <is>
           <t>Tochterunternehmen TU2</t>
         </is>
       </c>
-      <c r="B5" s="7" t="inlineStr">
+      <c r="B5" s="3" t="inlineStr">
         <is>
           <t>USD</t>
         </is>
@@ -3909,12 +3928,12 @@
           <t>0.9150</t>
         </is>
       </c>
-      <c r="E5" s="7" t="inlineStr">
+      <c r="E5" s="3" t="inlineStr">
         <is>
           <t>2024-12-31</t>
         </is>
       </c>
-      <c r="F5" s="7" t="inlineStr">
+      <c r="F5" s="3" t="inlineStr">
         <is>
           <t>Ausländische Tochter - Beispiel</t>
         </is>
@@ -3971,165 +3990,165 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="5" t="inlineStr">
+      <c r="A2" s="1" t="inlineStr">
         <is>
           <t>Unternehmen</t>
         </is>
       </c>
-      <c r="B2" s="5" t="inlineStr">
+      <c r="B2" s="1" t="inlineStr">
         <is>
           <t>Steuerart</t>
         </is>
       </c>
-      <c r="C2" s="5" t="inlineStr">
+      <c r="C2" s="1" t="inlineStr">
         <is>
           <t>Ursprung</t>
         </is>
       </c>
-      <c r="D2" s="5" t="inlineStr">
+      <c r="D2" s="1" t="inlineStr">
         <is>
           <t>Temporäre Differenz</t>
         </is>
       </c>
-      <c r="E2" s="5" t="inlineStr">
+      <c r="E2" s="1" t="inlineStr">
         <is>
           <t>Steuersatz (%)</t>
         </is>
       </c>
-      <c r="F2" s="5" t="inlineStr">
+      <c r="F2" s="1" t="inlineStr">
         <is>
           <t>Latente Steuer</t>
         </is>
       </c>
-      <c r="G2" s="5" t="inlineStr">
+      <c r="G2" s="1" t="inlineStr">
         <is>
           <t>HGB-Position</t>
         </is>
       </c>
-      <c r="H2" s="5" t="inlineStr">
+      <c r="H2" s="1" t="inlineStr">
         <is>
           <t>Bemerkung</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="6" t="inlineStr">
+      <c r="A3" s="2" t="inlineStr">
         <is>
           <t>Mutterunternehmen H</t>
         </is>
       </c>
-      <c r="B3" s="7" t="inlineStr">
+      <c r="B3" s="3" t="inlineStr">
         <is>
           <t>Aktiv</t>
         </is>
       </c>
-      <c r="C3" s="7" t="inlineStr">
+      <c r="C3" s="3" t="inlineStr">
         <is>
           <t>Bilanzierungshilfen</t>
         </is>
       </c>
-      <c r="D3" s="8" t="inlineStr">
+      <c r="D3" s="4" t="inlineStr">
         <is>
           <t>50000.00</t>
         </is>
       </c>
-      <c r="E3" s="8" t="inlineStr">
+      <c r="E3" s="4" t="inlineStr">
         <is>
           <t>25.00</t>
         </is>
       </c>
-      <c r="F3" s="9">
+      <c r="F3" s="5">
         <f>D3*E3/100</f>
         <v/>
       </c>
-      <c r="G3" s="7" t="inlineStr">
+      <c r="G3" s="3" t="inlineStr">
         <is>
           <t>D</t>
         </is>
       </c>
-      <c r="H3" s="7" t="inlineStr">
+      <c r="H3" s="3" t="inlineStr">
         <is>
           <t>Aktive latente Steuern</t>
         </is>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="6" t="inlineStr">
+      <c r="A4" s="2" t="inlineStr">
         <is>
           <t>Mutterunternehmen H</t>
         </is>
       </c>
-      <c r="B4" s="7" t="inlineStr">
+      <c r="B4" s="3" t="inlineStr">
         <is>
           <t>Passiv</t>
         </is>
       </c>
-      <c r="C4" s="7" t="inlineStr">
+      <c r="C4" s="3" t="inlineStr">
         <is>
           <t>Bewertungsunterschiede</t>
         </is>
       </c>
-      <c r="D4" s="8" t="inlineStr">
+      <c r="D4" s="4" t="inlineStr">
         <is>
           <t>30000.00</t>
         </is>
       </c>
-      <c r="E4" s="8" t="inlineStr">
+      <c r="E4" s="4" t="inlineStr">
         <is>
           <t>25.00</t>
         </is>
       </c>
-      <c r="F4" s="9">
+      <c r="F4" s="5">
         <f>D4*E4/100</f>
         <v/>
       </c>
-      <c r="G4" s="7" t="inlineStr">
+      <c r="G4" s="3" t="inlineStr">
         <is>
           <t>E</t>
         </is>
       </c>
-      <c r="H4" s="7" t="inlineStr">
+      <c r="H4" s="3" t="inlineStr">
         <is>
           <t>Passive latente Steuern</t>
         </is>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="6" t="inlineStr">
+      <c r="A5" s="2" t="inlineStr">
         <is>
           <t>Tochterunternehmen TU1</t>
         </is>
       </c>
-      <c r="B5" s="7" t="inlineStr">
+      <c r="B5" s="3" t="inlineStr">
         <is>
           <t>Aktiv</t>
         </is>
       </c>
-      <c r="C5" s="7" t="inlineStr">
+      <c r="C5" s="3" t="inlineStr">
         <is>
           <t>Abschreibungen</t>
         </is>
       </c>
-      <c r="D5" s="8" t="inlineStr">
+      <c r="D5" s="4" t="inlineStr">
         <is>
           <t>20000.00</t>
         </is>
       </c>
-      <c r="E5" s="8" t="inlineStr">
+      <c r="E5" s="4" t="inlineStr">
         <is>
           <t>25.00</t>
         </is>
       </c>
-      <c r="F5" s="9">
+      <c r="F5" s="5">
         <f>D5*E5/100</f>
         <v/>
       </c>
-      <c r="G5" s="7" t="inlineStr">
+      <c r="G5" s="3" t="inlineStr">
         <is>
           <t>D</t>
         </is>
       </c>
-      <c r="H5" s="7" t="inlineStr">
+      <c r="H5" s="3" t="inlineStr">
         <is>
           <t>Aktive latente Steuern</t>
         </is>

</xml_diff>

<commit_message>
Fix TypeScript build errors for Railway deployment
</commit_message>
<xml_diff>
--- a/templates/Konsolidierung_Muster_v3.0.xlsx
+++ b/templates/Konsolidierung_Muster_v3.0.xlsx
@@ -8,7 +8,7 @@
   </bookViews>
   <sheets>
     <sheet name="Bilanzdaten" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Anleitung1" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Anleitung" sheetId="2" state="visible" r:id="rId2"/>
     <sheet name="GuV-Daten" sheetId="3" state="visible" r:id="rId3"/>
     <sheet name="Unternehmensinformationen" sheetId="4" state="visible" r:id="rId4"/>
     <sheet name="Beteiligungsverhältnisse" sheetId="5" state="visible" r:id="rId5"/>
@@ -18,7 +18,6 @@
     <sheet name="Latente Steuern" sheetId="9" state="visible" r:id="rId9"/>
     <sheet name="HGB-Bilanzstruktur" sheetId="10" state="visible" r:id="rId10"/>
     <sheet name="Kontenplan-Referenz" sheetId="11" state="visible" r:id="rId11"/>
-    <sheet name="Anleitung" sheetId="12" state="visible" r:id="rId12"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -1904,24 +1903,6 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>

</xml_diff>